<commit_message>
added a lot of documentation and comments
</commit_message>
<xml_diff>
--- a/regulations outputs/in family connection statistics test old.xlsx
+++ b/regulations outputs/in family connection statistics test old.xlsx
@@ -12,8 +12,9 @@
     <sheet name="Modularity_based_communities" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Louvain_Communities" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Fluid_Communities" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Label_propagation" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Centrality_Communities" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Divisive_Communities" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Label_propagation" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Centrality_Communities" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -431,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -465,10 +466,15 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Divisive Communities</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Label propagation</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Centrality Communities</t>
         </is>
@@ -493,9 +499,12 @@
         <v>20</v>
       </c>
       <c r="F2" t="n">
+        <v>20</v>
+      </c>
+      <c r="G2" t="n">
         <v>2</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>20</v>
       </c>
     </row>
@@ -506,22 +515,25 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>50.35</v>
+        <v>14.9</v>
       </c>
       <c r="C3" t="n">
-        <v>142.5714285714286</v>
+        <v>41.85714285714285</v>
       </c>
       <c r="D3" t="n">
-        <v>142.5714285714286</v>
+        <v>41.85714285714285</v>
       </c>
       <c r="E3" t="n">
-        <v>49.9</v>
+        <v>14.65</v>
       </c>
       <c r="F3" t="n">
-        <v>499</v>
+        <v>14.65</v>
       </c>
       <c r="G3" t="n">
-        <v>49.9</v>
+        <v>146.5</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14.65</v>
       </c>
     </row>
     <row r="4">
@@ -531,21 +543,24 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>38.5</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>102</v>
+        <v>51</v>
       </c>
       <c r="D4" t="n">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="E4" t="n">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F4" t="n">
-        <v>499</v>
+        <v>2</v>
       </c>
       <c r="G4" t="n">
+        <v>146.5</v>
+      </c>
+      <c r="H4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -556,22 +571,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>38.78588321596023</v>
+        <v>10.18719526505805</v>
       </c>
       <c r="C5" t="n">
-        <v>139.0705542076361</v>
+        <v>33.33880907405347</v>
       </c>
       <c r="D5" t="n">
-        <v>77.33015182289752</v>
+        <v>19.16097223897726</v>
       </c>
       <c r="E5" t="n">
-        <v>31.32831240100138</v>
+        <v>4.51051403302387</v>
       </c>
       <c r="F5" t="n">
-        <v>701.4499269370551</v>
+        <v>50.23971484163124</v>
       </c>
       <c r="G5" t="n">
-        <v>215.1601362021467</v>
+        <v>204.3538597629122</v>
+      </c>
+      <c r="H5" t="n">
+        <v>59.86939733154247</v>
       </c>
     </row>
     <row r="6">
@@ -581,22 +599,25 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>34.25</v>
+        <v>9.5</v>
       </c>
       <c r="C6" t="n">
-        <v>246</v>
+        <v>63</v>
       </c>
       <c r="D6" t="n">
-        <v>95.5</v>
+        <v>25.5</v>
       </c>
       <c r="E6" t="n">
-        <v>33</v>
+        <v>7.5</v>
       </c>
       <c r="F6" t="n">
-        <v>496</v>
+        <v>3</v>
       </c>
       <c r="G6" t="n">
-        <v>2</v>
+        <v>144.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -623,6 +644,9 @@
       <c r="G7" t="n">
         <v>293</v>
       </c>
+      <c r="H7" t="n">
+        <v>293</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -631,22 +655,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.298152725300869</v>
+        <v>1.462620437943976</v>
       </c>
       <c r="C8" t="n">
-        <v>1.025173368897097</v>
+        <v>1.255508040619211</v>
       </c>
       <c r="D8" t="n">
-        <v>1.843671908183336</v>
+        <v>2.184499947867835</v>
       </c>
       <c r="E8" t="n">
-        <v>1.592808427127565</v>
+        <v>3.247966837646345</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7113836367179178</v>
+        <v>0.2916019735816703</v>
       </c>
       <c r="G8" t="n">
-        <v>0.2319202844950706</v>
+        <v>0.7168937262548735</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.2446993063730338</v>
       </c>
     </row>
     <row r="9">
@@ -656,22 +683,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.124087591240876</v>
+        <v>1.263157894736842</v>
       </c>
       <c r="C9" t="n">
-        <v>0.4146341463414634</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="D9" t="n">
-        <v>1.633507853403141</v>
+        <v>1.294117647058824</v>
       </c>
       <c r="E9" t="n">
-        <v>1.121212121212121</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
-        <v>1.006048387096774</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G9" t="n">
-        <v>0.5</v>
+        <v>1.013840830449827</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -687,15 +717,18 @@
         <v>1812</v>
       </c>
       <c r="D10" t="n">
-        <v>1619</v>
+        <v>1701</v>
       </c>
       <c r="E10" t="n">
-        <v>1133</v>
+        <v>1115</v>
       </c>
       <c r="F10" t="n">
+        <v>2872</v>
+      </c>
+      <c r="G10" t="n">
         <v>3165</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>3109</v>
       </c>
     </row>
@@ -712,15 +745,18 @@
         <v>1355</v>
       </c>
       <c r="D11" t="n">
-        <v>1548</v>
+        <v>1466</v>
       </c>
       <c r="E11" t="n">
-        <v>2034</v>
+        <v>2052</v>
       </c>
       <c r="F11" t="n">
+        <v>295</v>
+      </c>
+      <c r="G11" t="n">
         <v>2</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>58</v>
       </c>
     </row>
@@ -737,15 +773,18 @@
         <v>0.5721502999684244</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5112093463845911</v>
+        <v>0.5371013577518156</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3577518155983581</v>
+        <v>0.3520682033470161</v>
       </c>
       <c r="F12" t="n">
+        <v>0.9068519103252289</v>
+      </c>
+      <c r="G12" t="n">
         <v>0.9993684875276286</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>0.9816861383012314</v>
       </c>
     </row>
@@ -762,15 +801,18 @@
         <v>0.5018879211466615</v>
       </c>
       <c r="D13" t="n">
-        <v>0.4903660128347348</v>
+        <v>0.4965689769625984</v>
       </c>
       <c r="E13" t="n">
-        <v>0.3407183691053611</v>
+        <v>0.3381885992237573</v>
       </c>
       <c r="F13" t="n">
+        <v>0.283225557162202</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.8331753055204383</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>0.1645524296675192</v>
       </c>
     </row>
@@ -787,15 +829,18 @@
         <v>0.09721030042918455</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1174720650123349</v>
+        <v>0.1200084662057288</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2625115848007414</v>
+        <v>0.25421796625627</v>
       </c>
       <c r="F14" t="n">
+        <v>0.05527754253599199</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.03750355483932126</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>0.0431194696402319</v>
       </c>
     </row>
@@ -812,15 +857,18 @@
         <v>0.1882305960895143</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1291724033387157</v>
+        <v>0.1259806711449319</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2557749888999888</v>
+        <v>0.261857296255516</v>
       </c>
       <c r="F15" t="n">
+        <v>0.6099981118214579</v>
+      </c>
+      <c r="G15" t="n">
         <v>0.5187403720820002</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>0.7571667683885406</v>
       </c>
     </row>
@@ -837,15 +885,18 @@
         <v>0.02024926773865742</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02156769860952434</v>
+        <v>0.0205373903785268</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02503692762186115</v>
+        <v>0.02528027596402612</v>
       </c>
       <c r="F16" t="n">
+        <v>0.008779761904761905</v>
+      </c>
+      <c r="G16" t="n">
         <v>0.001718213058419244</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>0.004310985580496507</v>
       </c>
     </row>
@@ -862,15 +913,18 @@
         <v>0.01635676483684854</v>
       </c>
       <c r="D17" t="n">
-        <v>0.02102074355261216</v>
+        <v>0.01941221315769853</v>
       </c>
       <c r="E17" t="n">
-        <v>0.02450799564417745</v>
+        <v>0.02458451519778011</v>
       </c>
       <c r="F17" t="n">
+        <v>0.006139402141691993</v>
+      </c>
+      <c r="G17" t="n">
         <v>0.001718213058419244</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.004329972156146078</v>
       </c>
     </row>
@@ -887,15 +941,18 @@
         <v>0.6552129715014351</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6897621508019659</v>
+        <v>0.7077481915489288</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8258594529950826</v>
+        <v>0.8191024332517941</v>
       </c>
       <c r="F18" t="n">
+        <v>0.7258778844532167</v>
+      </c>
+      <c r="G18" t="n">
         <v>0.9123847215199992</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>0.8182186715082385</v>
       </c>
     </row>
@@ -912,15 +969,18 @@
         <v>0.8400999478874375</v>
       </c>
       <c r="D19" t="n">
-        <v>0.720083852190384</v>
+        <v>0.7329688691326508</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8251196326881161</v>
+        <v>0.8283454843896728</v>
       </c>
       <c r="F19" t="n">
+        <v>0.9800713249800299</v>
+      </c>
+      <c r="G19" t="n">
         <v>0.99339731111187</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>0.9886277329222739</v>
       </c>
     </row>
@@ -937,15 +997,18 @@
         <v>0.7610834937156346</v>
       </c>
       <c r="D20" t="n">
-        <v>0.7154228964427142</v>
+        <v>0.7234522416255024</v>
       </c>
       <c r="E20" t="n">
-        <v>0.823241160387451</v>
+        <v>0.8267029253671794</v>
       </c>
       <c r="F20" t="n">
+        <v>0.9443570584316672</v>
+      </c>
+      <c r="G20" t="n">
         <v>0.9544516023320979</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>0.9620527569504668</v>
       </c>
     </row>
@@ -960,7 +1023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1022,11 +1085,6 @@
           <t>inner connections probability</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1065,17 +1123,6 @@
       <c r="J2" t="n">
         <v>0.2404692082111437</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>**General Topic: Access Control and Information Flow Management**
-Here's a summary of the provided regulations in concise bullet points:
-*   **Access Control Policies and Account Management:** Establish and maintain policies for access control, including account creation, management, monitoring, and termination, as well as the use of privileged accounts. Enforce account reviews and ensure alignment with personnel changes.
-*   **Access Enforcement Mechanisms:** Enforce access authorizations using various methods like mandatory, discretionary, role-based, and attribute-based access control. Implement controls for dual authorization, revocation, and auditing overrides.
-*   **Information Flow Controls:** Manage the flow of information within and between systems through policies that enforce security and privacy attributes, protected processing domains, dynamic controls, filters, data sanitization, and metadata validations.
-*   **Least Privilege and Separation of Duties:** Implement the principles of least privilege, ensuring users only have the necessary access for their roles and separating duties to prevent unauthorized actions. Restrict privileged access to authorized personnel only.
-*   **Session Management, Remote and Wireless Access, and Device Controls:** Manage user sessions, enforcing limits on login attempts and implementing lockouts, logouts, and notifications. Establish and control secure remote and wireless access and implement security for mobile devices. Additionally, manage the sharing of information, publicly accessible content, and data mining protection, and set up access control decisions.</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1112,17 +1159,6 @@
       <c r="J3" t="n">
         <v>0.09090909090909091</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **Security and Privacy Training and Awareness**.
-Here's a summary of the regulations in bullet points:
-*   **Establish a Formal Training Program:** Organizations must develop, document, and disseminate a security and privacy awareness and training policy and procedures.
-*   **Provide Comprehensive Literacy Training:**  Provide regular security and privacy literacy training to all system users, covering general threats, insider threats, social engineering, and more.
-*   **Offer Role-Based Training:** Deliver role-specific training to personnel based on their responsibilities, including environmental controls, physical security, and PII processing.
-*   **Incorporate Practical Exercises:** Include practical exercises in both literacy and role-based training to simulate incidents and reinforce learning.
-*   **Maintain and Monitor Training Activities:** Document training activities, retain individual training records, update content regularly, and provide feedback on training results.</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1160,16 +1196,6 @@
       <c r="J4" t="n">
         <v>0.3554502369668247</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>**General Topic:** System Auditing and Accountability
-*   **Comprehensive Audit Policy &amp; Procedures:** Organizations must develop, document, and disseminate a detailed audit and accountability policy and associated procedures, which should be reviewed and updated regularly.
-*   **Robust Event Logging &amp; Content:**  Organizations must log specific system events with detailed information, including what happened, when, where, and by whom, and must allocate sufficient storage for those logs.
-*   **Failure Response Mechanisms:**  Organizations must have processes to respond to failures in the audit logging process, including real-time alerts and potential system shutdowns, with alternate logging capabilities.
-*   **Analysis, Review &amp; Reporting:**  Organizations must regularly review, analyze, and report on audit records, integrating with other data sources to enhance the ability to identify suspicious activity and adjusting level of review based on risks.
-*   **Protection of Audit Data &amp; Non-repudiation:** Organizations must protect audit data from unauthorized access, use cryptographic mechanisms, implement dual authorization for critical actions, use write-once media where appropriate, and establish methods to prove actions were performed (non-repudiation).</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1206,16 +1232,6 @@
       <c r="J5" t="n">
         <v>0.1120689655172414</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **System Security Assessment, Authorization, and Monitoring**. Here's a summary:
-*   **Policy and Procedures:** Organizations must establish and maintain policies and procedures for assessing, authorizing, and monitoring their systems, including designating a responsible official and regularly reviewing these documents.
-*   **Control Assessments:**  Regular, documented control assessments must be conducted, and when possible by independent assessors, to verify the effectiveness of security and privacy controls; these results must be reported to designated personnel, and may include specialized forms of testing such as penetration tests. Organizations may also leverage external assessments if they meet specific requirements.
-*   **Information Exchange:**  Agreements must be in place to manage information exchange between systems, defining interface characteristics, security requirements, and responsibilities. Data transfers should be authorized, and transitive information exchanges must be identified and managed.
-*   **Authorization and Remediation:** Systems require formal authorization by a designated senior official before operation, including joint authorization processes as needed.  Organizations must also develop and maintain Plans of Action and Milestones (POAMs) to address weaknesses or deficiencies discovered.
-*   **Continuous Monitoring:** Organizations must implement continuous monitoring strategies, including metrics, assessments, and responses to identified issues, along with ongoing independent assessments, trend analysis, and risk monitoring, with automation to ensure accuracy and availability of monitoring results.</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1253,16 +1269,6 @@
       <c r="J6" t="n">
         <v>0.2301255230125523</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **System and Configuration Management**. Here's a summary:
-*   **Configuration Control:** Establish policies, baselines, and change management processes to control system configurations, including change documentation, approvals, testing, and automated implementation, with particular emphasis on security and privacy impacts.
-*   **Component Inventory:** Develop and maintain an accurate and up-to-date inventory of all system components, including hardware, software, and firmware. This inventory should include locations, responsible parties, and authorized configurations, tracked through automated methods with alerts for unauthorized components.
-*   **Least Functionality &amp; Software:** Configure systems to only provide essential capabilities by restricting or prohibiting unnecessary functions, ports, and protocols. Manage software usage by restricting or prohibiting unauthorized software, governing user-installed software, and implementing usage restrictions for software, open-source or otherwise.
-*   **Access Restrictions:** Enforce strict physical and logical access controls for system changes, using automated tools, dual authorization, and privilege limitation. Regularly review and manage access privileges, especially for sensitive or operational system environments.
-*   **Information &amp; Data Management**:  Identify, document, and track the location of information and system components involved in processing and storing data, and create data action maps. Also, implement signing requirements to ensure only authenticated components are installed.</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1300,16 +1306,6 @@
       <c r="J7" t="n">
         <v>0.3496503496503496</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>**General Topic:** System Contingency Planning and Disaster Recovery
-*   **Comprehensive Contingency Planning:** Organizations must develop, document, and maintain a detailed contingency plan that covers essential functions, recovery objectives, roles/responsibilities, and full system restoration. The plan must also include coordination with incident response.
-*   **Alternate Site and Service Preparedness:** Organizations are required to have alternate processing and storage sites, and telecommunications services, with agreements that ensure timely transfer and resumption of operations. These resources must be tested, separated from primary sites, and prioritized for service.
-*   **Robust Backup and Recovery:** Regulations mandate regular backups of user, system, and documentation data, as well as testing the reliability of these backups. Backup information should be securely stored, and dual authorization is required for deletion.
-*   **Regular Testing and Training:** Contingency plans must be regularly tested, including full system recovery and reconstitution, using simulated events to provide realistic training. Training should be provided to personnel based on assigned roles and frequency.
-*  **System Resilience Measures:** Organizations must implement measures like safe mode, alternative security mechanisms and alternative communication protocols to enhance system resilience during disruptions and to ensure continuity of operations</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1347,16 +1343,6 @@
       <c r="J8" t="n">
         <v>0.3488372093023256</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>**Topic:** Identity and Access Management
-*   **Policy and Procedures:** Organizations must establish and maintain policies and procedures for identification and authentication, including management responsibilities and periodic review.
-*   **User and Device Authentication:**  Regulations mandate unique identification and authentication for all users and devices, with multi-factor authentication required for privileged and non-privileged accounts.
-*   **Authenticator Management:**  Detailed requirements for managing authenticators including password complexity, cryptographic key management, handling of default authenticators and biometric security are laid out.
-*  **Identifier Management:** Rules about assignment, uniqueness, and protection of user and system identifiers are specified along with how to handle dynamic identifiers.
-*  **Identity Proofing:**  Regulations outline the process for verifying user identities before granting system access including in-person validation and the use of external identity verification.</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1393,16 +1379,6 @@
       <c r="J9" t="n">
         <v>0.2641509433962264</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>**General Topic:** Incident Response Management
-*   **Policy &amp; Procedures:** Establish and maintain a documented incident response policy and procedures, including designated roles, responsibilities, regular reviews, and updates.
-*   **Training &amp; Testing:** Implement comprehensive incident response training programs, including simulated events, automated environments, and breach scenarios; Conduct regular and automated testing of incident response capabilities.
-*   **Incident Handling:** Develop a robust incident handling capability covering preparation, detection, analysis, containment, eradication, recovery, and continuous improvement; include automated processes, dynamic reconfiguration, continuity of operations, information correlation, and handling of insider threats.
-*  **Incident Monitoring &amp; Reporting:** Track and document all incidents using automated mechanisms; Require personnel to report incidents within a set timeframe; Report vulnerabilities and information to relevant authorities.
-*   **Incident Response Support:** Establish a dedicated incident response support resource for advice and assistance; Coordinate with external providers and build direct relationships. Develop a comprehensive incident response plan, including handling of breaches, information spillage, and ensuring continuity of operations.</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1439,17 +1415,6 @@
       <c r="J10" t="n">
         <v>0.12</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **System Maintenance**.
-Here's a summary of the regulations in bullet points:
-*   **Establish comprehensive maintenance policies and procedures**: Organizations must develop and maintain documented policies and procedures covering all aspects of system maintenance, including roles, responsibilities, and compliance with regulations.
-*   **Implement controlled maintenance practices:**  Maintenance activities (both on-site and remote) require approval, monitoring, and documentation, along with procedures for sanitizing equipment and verifying system functionality post-maintenance.
-*   **Control and secure maintenance tools:** Organizations must manage maintenance tools, including approval, regular inspection, restrictions on use, and ensuring software is up to date, while also preventing unauthorized removal or modifications.
-*   **Secure remote (nonlocal) maintenance sessions:** Nonlocal maintenance requires strong authentication, session protection (with cryptographic protection, and separation), approvals, notifications, logging/review, and termination verification. Additionally, ensure comparable security practices as systems being serviced.
-*   **Establish maintenance personnel requirements**: Organizations must authorize personnel and ensure they possess appropriate security clearances, access authorizations, and citizenship status while also outlining requirements for personnel lacking these measures (i.e. escorts, sanitization).</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1485,16 +1450,6 @@
       </c>
       <c r="J11" t="n">
         <v>0.1232876712328767</v>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>**General Topic:** Media Protection and Handling
-*   **Policy and Procedures:** Organizations must create, document, and disseminate media protection policies and procedures, including designated personnel and regular review processes.
-*   **Access Control:** Access to digital and non-digital media must be restricted to authorized personnel.
-*   **Media Handling:** Media must be marked with handling caveats, securely stored in controlled areas, and protected during transport, using defined controls and custodians.
-*   **Sanitization and Disposal:** Media must be sanitized before disposal, release, or reuse, utilizing appropriate techniques that are tested and verified, including considerations for portable devices.
-*   **Media Use and Downgrading:** Organizations need to control media use, prohibit sanitization-resistant media, establish a downgrading process, and document all related actions for controlled and classified information.</t>
-        </is>
       </c>
     </row>
     <row r="12">
@@ -1534,16 +1489,6 @@
       <c r="J12" t="n">
         <v>0.2595419847328244</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>**General Topic:** Physical and Environmental Protection
-*   **Policy and Access Control:** Establish policies and procedures for physical and environmental protection, including access authorizations based on role/position, and implement controls for physical access to the facility and system. This includes requiring two forms of ID for visitors and restricting unescorted access.
-*   **Monitoring and Surveillance:** Implement monitoring of physical access using logs, intrusion alarms, and video surveillance, as well as maintain visitor access records and report anomalies.
-*   **Power and Emergency Systems:** Protect power equipment and cabling, provide emergency power and lighting, and ensure emergency shutoff capabilities. These should be supported by a backup energy source in case of an outage.
-*   **Fire and Environmental Controls:** Employ fire detection and suppression systems, maintain environmental controls (temperature, humidity etc.) with automatic adjustments and alarms, and protect against water damage.
-*   **Asset and Component Protection:** Control delivery and removal of system components, protect against information leakage, monitor asset locations, and mark hardware components with their impact level. Ensure system components are located in areas with minimal potential damage.</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1579,17 +1524,6 @@
       </c>
       <c r="J13" t="n">
         <v>0.1276595744680851</v>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **System Security and Privacy Governance and Planning**.
-Here's a summary of the regulations in bullet points:
-*   **Establish Core Security Documentation:** Organizations must develop and maintain key documents, including a planning policy, system security and privacy plans, a concept of operations (CONOPS), and security and privacy architectures.
-*   **Define User Responsibilities:** Rules of behavior must be created and acknowledged by all users, with restrictions in place for social media, external sites, and organization credentials.
-*   **Implement Structured Planning and Management:** There must be designated personnel managing the documentation, plans, and architectures that also need regular reviews and updates based on defined frequencies and changes.
-*   **Implement Security and Privacy Controls:** The system architectures must implement defense in depth, using diversified suppliers, and have centrally managed controls, and based on tailored baselines.
-*   **Ensure Integration and Coordination:** The plans and architectures should be integrated into the broader enterprise architecture with defined dependencies and coordination, and all plans and policies should be approved before implementation.</t>
-        </is>
       </c>
     </row>
     <row r="14">
@@ -1630,16 +1564,6 @@
       <c r="J14" t="n">
         <v>0.2139917695473251</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>**General Topic: Comprehensive Cybersecurity and Privacy Program Management**
-*   **Establish Formal Programs:** Organizations must develop and maintain formal, documented information security and privacy programs, including specific plans, leadership roles, and resource allocation.
-*   **Risk Management Focus:**  A core element is a strong risk management approach, encompassing system-level security, privacy risks related to personally identifiable information (PII), and supply chain risk management. This includes strategy development, implementation, review, and consistent application across the organization.
-*   **Continuous Monitoring and Improvement:**  Organizations must continuously monitor security and privacy controls, track performance using defined metrics, and make necessary adjustments to respond to identified risks. Regular testing, training and monitoring are required.
-*   **Data Governance and PII Protection:** Stringent requirements for managing PII throughout its lifecycle, including inventorying systems that handle PII, controlling disclosures, ensuring accuracy, limiting use for non-mission purposes and establishing processes for handling complaints and appeals.
-*   **Proactive Threat Management and Information Sharing:** Implement a cross-discipline insider threat program and a broader threat awareness program with automated information sharing to enhance overall security posture, as well as, fostering external collaboration with security and privacy groups.</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1676,17 +1600,6 @@
       <c r="J15" t="n">
         <v>0.3387096774193548</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **Personnel Security and Access Control.**
-Here's a summary of the regulations:
-*   **Policy and Procedures:** Organizations must develop, document, and disseminate personnel security policies and procedures, assigning responsibility and ensuring regular reviews and updates.
-*   **Personnel Screening:** Individuals must be screened before gaining system access, with specific requirements for classified information, special protection information, and citizenship, also including rescreening policies.
-*   **Access Management:** Access agreements must be developed, signed, and re-signed as required. Special rules exist for access to classified information and post-employment requirements.
-*   **Personnel Termination/Transfer:** System access must be disabled upon termination, authenticators revoked, and exit interviews must be conducted. Transfer of personnel requires review of current access and updates if necessary.
-*   **External Personnel and Sanctions:**  Personnel security requirements must be established and followed for external providers. A formal sanctions process for personnel who don't comply with policies needs to be in place and security roles need to be incorporated into position descriptions.</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -1723,16 +1636,6 @@
       <c r="J16" t="n">
         <v>0.2876712328767123</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>**General Topic:** Personally Identifiable Information (PII) Processing and Privacy
-*   **Policy and Procedures:** Organizations must establish, document, and regularly update policies and procedures for PII processing, designating a responsible official.
-*   **Authorization and Purpose:** PII processing must be explicitly authorized, with data tagged accordingly, and restricted to compatible, documented purposes.
-*   **Consent Management:**  Organizations need to implement mechanisms for individuals to give, tailor, and revoke consent for PII processing, including 'just-in-time' consent.
-*   **Transparency and Notice:**  Organizations need to provide clear and accessible privacy notices to individuals, including Privacy Act statements, system of record notices, and routine uses.
-*   **Specific PII Handling:**  Specific categories of PII like Social Security Numbers and First Amendment data require additional protections, with limitations on use and disclosure, and specific rules for computer matching.</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -1769,16 +1672,6 @@
       <c r="J17" t="n">
         <v>0.1904761904761905</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>**General Topic: Risk Management and Vulnerability Assessment**
-*   **Risk Assessment Policies and Procedures:** Organizations must develop, document, and maintain risk assessment policies and procedures, including regular reviews and updates. This includes defining roles, responsibilities and integrating risk assessments across the organization.
-*   **System Categorization and Prioritization:** Systems and information must be categorized based on security impact and criticality, documented, and approved by authorized officials.
-*   **Comprehensive Risk Assessment:** Conduct regular risk assessments, identify vulnerabilities and threats, determine potential impacts, and integrate results. This process includes supply chain risks, threat intelligence, and predictive analytics.
-*   **Vulnerability Management:** Implement regular vulnerability monitoring and scanning, using automated tools, and remediate findings based on risk. This includes establishing public reporting channels and implementing access controls for scanning activities.
-*   **Proactive Security Measures:** Implement threat hunting capabilities to identify and disrupt threats evading existing controls. Conduct technical surveillance countermeasures surveys regularly, and perform privacy impact assessments.</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
@@ -1815,17 +1708,6 @@
       </c>
       <c r="J18" t="n">
         <v>0.2642276422764228</v>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations, categorized by the general topic and presented in concise bullet points:
-**General Topic:** Secure System and Service Acquisition and Development
-*   **Policy and Planning:** Organizations must establish and maintain documented policies, procedures, and assigned responsibilities for system acquisition, allocating sufficient resources for security and privacy and embedding security into the system development life cycle.
-*   **Secure Development Practices:** Regulations emphasize the need for secure system development, requiring the use of a defined system development lifecycle, secure coding practices, the implementation of security and privacy engineering principles, and the inclusion of security requirements into the acquisition process.
-*   **Rigorous Testing and Verification:** The regulations mandate comprehensive testing and evaluation, including static and dynamic analysis, threat modeling, penetration testing, and independent verification to ensure control effectiveness and flaw remediation.
-*   **Supply Chain Security:** Organizations must ensure that external service providers and developers comply with organizational security requirements and establish trust relationships, and maintain exclusive control of cryptographic keys when using external systems.
-*   **Configuration Management and Documentation:**  Regulations require configuration management throughout the system lifecycle, documentation of secure configurations, and the provision of administrator and user documentation for secure system operation as well as ensuring hardware and software integrity through configuration management processes.</t>
-        </is>
       </c>
     </row>
     <row r="19">
@@ -1868,17 +1750,6 @@
       <c r="J19" t="n">
         <v>0.3434903047091413</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>This group of cyber regulations covers **System and Communications Protection**.
-Here's a summary in bullet points:
-*   **Establish and Maintain Policies:** Organizations must develop, document, and regularly update policies and procedures for system and communications protection, designating a responsible official.
-*   **Implement Security Function Isolation:** Separate user and system functionalities, isolate security functions from non-security ones using hardware and layered structures, and minimize non-security functionality within the security boundary. 
-*   **Control Information Flow:** Prevent unauthorized information transfer via shared resources, manage denial-of-service attacks, protect resource availability, and monitor communications at system boundaries.
-*   **Protect Data in Transit and at Rest:** Implement cryptographic mechanisms for data transmission and storage, manage cryptographic keys, protect session authenticity, and prevent unauthorized access, while also protecting information at rest.
-*   **Enforce Secure Configurations and Practices:** Implement secure practices with collaborative computing, enforce mobile code restrictions, use secure name/address resolution services,  employ anti-spoofing, and implement various mechanisms to prevent exploitation of vulnerabilities.</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
@@ -1917,17 +1788,6 @@
       <c r="J20" t="n">
         <v>0.160337552742616</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **System and Information Integrity**.
-Here's a summary of the regulations:
-*   **Establish Policies and Procedures:** Organizations must create, document, and disseminate policies and procedures to manage system and information integrity, including roles, responsibilities, and compliance with laws and regulations.
-*   **Remediate System Flaws:** Timely identification, reporting, and correction of system flaws is required, including testing updates before installation, using automated patch management tools, and often removing old versions of software after updates.
-*   **Protect Against Malicious Code:** Implement mechanisms (signature or non-signature) to detect and eradicate malicious code at entry/exit points, regularly updating these mechanisms, and also including detection of unauthorized commands.
-*   **Monitor Systems for Anomalies and Intrusions:** Regularly monitor systems, traffic (including wireless) for unauthorized connections, attacks, and other suspicious activities, and use automated tools and alerts to ensure a timely response. Also includes the need to correlate information from multiple monitoring sources to develop situational awareness and identify covert exfiltration.
-*   **Maintain Software, Firmware, and Information Integrity:** Employ tools to detect unauthorized changes, verify integrity during startup and events, manage information outputs, protect memory, implement fail-safe procedures and other processes to ensure the validity of system components, data, and Personally Identifiable Information (PII). PII elements should be minimized, de-identified, and properly handled across their life cycle.</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
@@ -1964,17 +1824,6 @@
       </c>
       <c r="J21" t="n">
         <v>0.2241379310344828</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **Supply Chain Risk Management (SCRM)**.
-Here's a summary of the regulations in short, concise bullet points:
-*   **Establish comprehensive SCRM policies and procedures:** Develop and maintain policies, plans, and a dedicated team to manage supply chain risks, including regular reviews and updates.
-*   **Implement supply chain controls:** Put in place diverse supply sources, and processes to identify and address supply chain weaknesses, including limitations on harm from adversaries and flow-down requirements to subcontractors.
-*   **Ensure supply chain integrity and provenance:** Document, track, validate, and authenticate the sources and components of critical systems and their associated data through unique identification and integrity validation.
-*  **Employ secure acquisition practices:** Use appropriate acquisition strategies, tools, methods and assessments for critical components, including supplier assessments, and operations security, with defined notification agreements.
-*   **Protect against and manage tampering and counterfeit components:** Implement measures to detect, prevent, and report counterfeit components. Include tamper protection programs, and specific disposal techniques.</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -1988,7 +1837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2050,11 +1899,6 @@
           <t>inner connections probability</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -2096,16 +1940,6 @@
       <c r="J2" t="n">
         <v>0.5979899497487438</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>**General Topic:** System Security and Configuration Management
-*   **Access and Device Control:** Manages concurrent sessions, mobile device access (especially with classified data), and encryption on mobile devices.
-*   **Audit and Non-Repudiation:** Focuses on protecting audit logs, ensuring non-repudiation through identity association, and establishing a chain of custody.
-*   **Configuration Management:** Encompasses baseline configurations, change control, impact analysis, access restrictions, and least functionality principles for systems.
-*   **Contingency and Recovery:** Addresses planning, training, testing, and alternate site requirements for business continuity, including backups and system restoration.
-*   **Monitoring and Protection:** Covers incident response, system monitoring, vulnerability scanning, denial-of-service protection, boundary security, and the integrity of software and firmware.</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -2147,18 +1981,6 @@
       <c r="J3" t="n">
         <v>0.6067677946324388</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations:
-**General Topic:** Access Control, Authentication, and Information Flow Management
-*   **Account and Identity Management:** Regulations focus on the complete lifecycle of user and device accounts, including creation, modification, disabling, monitoring, and removal. This includes privileged accounts, shared accounts, temporary accounts, and inactive accounts. Multi-factor authentication and strong password policies are emphasized.
-*   **Access Enforcement and Control:** Regulations require the enforcement of access control policies (mandatory, discretionary, role-based, attribute-based), dual authorization for sensitive actions, and the revocation of access authorizations when necessary. Access to security-relevant information is restricted.
-*   **Information Flow Control:** Regulations focus on controlling information flow within and between systems, including the use of security and privacy attributes, metadata, filters, data sanitization, and the separation of data flows. Controls are enforced for encrypted information and embedded data types.  There is also a focus on handling the transfer of data between security domains.
-*    **User and Device Controls:** Regulations include device locking, session termination, system use notifications,  rules of behavior, and the proper handling of user logons and logon failures.  Remote and wireless access is also covered, mandating the use of secure connections and strong authentication.
-*   **Personnel Management and Security:** Regulations cover personnel screening, termination, transfers, and the requirement for signed access agreements. There is a strong emphasis on maintenance personnel authorizations, restrictions based on nationality/security clearances, and non-local maintenance controls, as well as media handling and marking. These sections ensure that people with access to sensitive information are trustworthy and compliant with organizational policies and procedures.
-These regulations, as a whole, aim to establish a secure environment through a combination of robust access controls, strong identity management practices, and careful management of how information flows within and between systems. There are also requirements for detailed logging and auditing practices and incident response plans to ensure compliance.</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -2200,17 +2022,6 @@
       <c r="J4" t="n">
         <v>0.566320645905421</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Okay, here is a summary of the provided cyber regulations:
-**General Topic:** Comprehensive Cybersecurity and Privacy Program Management
-*   **Training and Awareness:**  Organizations must provide regular security and privacy training to all users, including specialized training for specific roles, and emphasize practical exercises, insider threats, social engineering, and current cyber threats, as well as documenting all training activities and results.
-*   **Risk Management &amp; Assessment:**  A comprehensive risk management strategy is needed including regular risk assessments, especially supply chain risks, and must be documented, reviewed and kept up-to-date, along with plans of action and milestones to remediate risks, also taking advantage of external risk information and leveraging independent assessors where needed.
-*   **System Authorization &amp; Monitoring:** Implement a formal authorization process with designated officials and a robust continuous monitoring program with defined metrics, independent assessment and reporting; and also use automated tools for monitoring and consider trend analysis and risk monitoring.
-*   **Secure Development &amp; Acquisition:** Employ a secure system development lifecycle, incorporating security and privacy principles, including documentation and regular testing and evaluation; and manage the supply chain via contract requirements and a security conscious acquisition process with strict configuration management and use of only approved components.
-*   **System &amp; Environment Protection:** Ensure physical and environmental security of systems with emergency shutoff capabilities; control access to and use of maintenance tools; and maintain detailed system documentation; with specific measures for tamper resistance and detection and controls in place for supply chain security.</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -2250,17 +2061,6 @@
       <c r="J5" t="n">
         <v>0.4819277108433735</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **Comprehensive Cybersecurity and Privacy Governance.**
-Here is a summary of the regulations in bullet points:
-*   **Establish and Maintain Policies &amp; Procedures:** Develop, document, disseminate, and regularly review and update a wide range of policies and procedures related to information security, privacy, and risk management including access control, awareness and training, incident response, and more, with assigned personnel responsible for their management.
-*   **Protect Data &amp; Systems:** Implement controls for data mining prevention, information location tracking, data action mapping, media sanitization, shared system resource protections, and prevent unauthorized sensor data collection/use.
-*   **Incident Response &amp; Spillage:** Develop incident response plans, provide training (including simulated events and breach handling), enforce incident reporting (including automated), coordinate with external providers, manage information spillage incidents, and implement post-spill operations.
-*    **Privacy &amp; Personally Identifiable Information (PII):** Create and maintain privacy program plans, establish accountability of PII disclosures, manage PII quality, appoint privacy leadership, define PII processing purposes, manage consent, provide privacy notices, and handle system of records documentation.
-*    **General Risk Management &amp; Program Oversight:** Appoint risk management leaders, conduct system inventories, implement complaint processes, establish data integrity boards, define and enforce risk assessments, manage supply chain risks, maintain information lifecycle controls, implement personnel sanctions, and implement de-identification processes where applicable.</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -2295,16 +2095,6 @@
       <c r="J6" t="n">
         <v>0.3809523809523809</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>**General Topic:** System and Security Architecture
-*   **Access Control and Isolation:** Implement reference monitors, separation of user and system functionalities, and various isolation techniques to control access and enforce security policies.
-*   **Security Function Isolation:** Isolate security functions from non-security functions using hardware and software mechanisms, layering, and by minimizing dependencies.
-*   **Trusted Path:** Establish a secure and distinguishable path for communication between users and trusted system components, particularly for sensitive functions like authentication.
-*   **System Partitioning:** Partition systems into separate domains (physical or logical), especially for privileged functions, to enhance security and restrict access.
-*   **Process Isolation:** Ensure each process and thread executes in separate, protected domains, leveraging hardware and software mechanisms to prevent interference and unauthorized access.</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -2339,16 +2129,6 @@
       <c r="J7" t="n">
         <v>0.3529411764705883</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>**General Topic:** Physical and Environmental Security &amp; Wireless Communications Security
-*   **Physical Security:** Regulations focus on protecting system components through strategic placement, facility planning, and implementing safeguards against physical and environmental threats like electromagnetic pulses.
-*   **Information Leakage:** Systems must be protected from information leakage due to electromagnetic emanations, adhering to national policies based on data sensitivity.
-*   **Asset Tracking:** Employ technologies to monitor the location of critical assets within defined areas.
-*   **Wireless Security:** Wireless links require cryptographic mechanisms to guard against attacks, interference, detection, and deceptive communications.
-*   **Critical Infrastructure:** Information security and privacy must be included in critical infrastructure protection plans.</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -2382,16 +2162,6 @@
       </c>
       <c r="J8" t="n">
         <v>0.5263157894736842</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>**Topic: System and Data Resiliency and Security**
-*   **Minimize System Footprint:** Implement thin nodes with minimal functionality and storage, focusing on essential operations.
-*   **Promote Diversity and Agility:** Utilize platform-independent applications and diverse technologies, including virtualization, to enhance system adaptability and resilience.
-*  **Employ Deception Techniques:** Use concealment, misdirection, and randomness to confuse adversaries, misleading them about system state and configuration.
-*   **Embrace Non-Persistence:** Implement non-persistent system components, services, and data, refreshing from trusted sources and deleting data when no longer required.
-*   **Regularly Refresh Data:** Refresh or generate data on demand at defined frequencies, deleting data when no longer needed to limit exposure and enhance security.</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -2405,7 +2175,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2467,59 +2237,45 @@
           <t>inner connections probability</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['AC-4' 'AC-25' 'CM-3' 'CM-5' 'CM-6' 'CM-8' 'CM-9' 'CM-10' 'CM-11' 'CM-12'
- 'CM-13' 'IA-9' 'PL-9' 'PM-16' 'PM-27' 'SC-5' 'SC-16' 'SC-18' 'SC-26'
- 'SC-28' 'SC-31' 'SC-34' 'SC-35' 'SC-37' 'SC-39' 'SC-40' 'SC-43' 'SC-44'
- 'SC-46' 'SC-49' 'SI-3' 'SI-4' 'SI-7' 'SI-8' 'SI-10' 'SI-11' 'SI-15'
- 'SI-16']</t>
+          <t>['AC-8' 'AU-2' 'AU-3' 'AU-4' 'AU-5' 'AU-6' 'AU-7' 'AU-8' 'AU-11' 'AU-12'
+ 'AU-14' 'CM-2' 'CM-3' 'CM-4' 'CM-5' 'CM-6' 'CM-7' 'CM-8' 'CM-9' 'CM-10'
+ 'CM-11' 'IR-4' 'IR-5' 'MA-2' 'MA-3' 'MA-4' 'MA-7' 'PE-6' 'PE-8' 'PE-16'
+ 'PL-9' 'PM-16' 'PM-30' 'RA-5' 'SA-10' 'SA-15' 'SC-5' 'SC-18' 'SC-25'
+ 'SC-26' 'SC-27' 'SC-29' 'SC-30' 'SC-31' 'SC-34' 'SC-35' 'SC-37' 'SC-44'
+ 'SI-2' 'SI-3' 'SI-4' 'SI-5' 'SI-6' 'SI-7' 'SI-8' 'SI-10' 'SI-11' 'SI-15'
+ 'SR-3' 'SR-4' 'SR-5' 'SR-6' 'SR-8' 'SR-9' 'SR-10' 'SR-11']</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1406</v>
+        <v>4290</v>
       </c>
       <c r="E2" t="n">
-        <v>170</v>
+        <v>542</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1209103840682788</v>
+        <v>0.1263403263403264</v>
       </c>
       <c r="G2" t="n">
-        <v>9690</v>
+        <v>14982</v>
       </c>
       <c r="H2" t="n">
-        <v>287</v>
+        <v>349</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02961816305469556</v>
+        <v>0.02329462021091977</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3719912472647702</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations:
-**General Topic:** System and Information Security Controls
-*   **Information Flow Control:** A primary focus is on enforcing policies to control the flow of information within and between systems, including dynamic flows, encrypted data, embedded data types, metadata, and the use of one-way mechanisms.
-*   **Configuration Management:** There are extensive requirements for configuration change control, including automated documentation, testing, and responses to unauthorized changes, along with limitations on user privileges.
-*   **System Monitoring and Integrity:**  Regulations mandate continuous system monitoring for attacks and anomalies, intrusion detection, and the use of integrity verification tools for software, firmware, and information with automated responses to violations.
-*   **Malicious Code Protection:**  Controls include implementing mechanisms to detect, eradicate, and update malicious code protection, as well as analysis of malicious code characteristics and behavior and taking actions on unauthorized operating system commands.
-*   **Access and Data Security:** Regulations cover user software restrictions, information location, data sanitization, access restrictions on system changes, cryptography, process isolation, memory protection, and protection of information at rest through multiple means such as encryption and offline storage.</t>
-        </is>
+        <v>0.6083052749719416</v>
       </c>
     </row>
     <row r="3">
@@ -2527,47 +2283,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['AC-7' 'AC-9' 'AC-11' 'AC-18' 'AC-19' 'AC-22' 'AC-24' 'AU-9' 'AU-10'
- 'AU-13' 'CA-9' 'CM-2' 'CM-14' 'IA-3' 'IA-7' 'MP-2' 'MP-4' 'MP-5' 'MP-7'
- 'PE-4' 'PE-9' 'PE-17' 'PL-4' 'SC-8' 'SC-12' 'SC-13' 'SC-15' 'SC-17'
- 'SC-41' 'SI-20']</t>
+          <t>['AC-2' 'AC-3' 'AC-4' 'AC-5' 'AC-6' 'AC-7' 'AC-9' 'AC-11' 'AC-14' 'AC-16'
+ 'AC-17' 'AC-18' 'AC-19' 'AC-20' 'AC-24' 'AU-9' 'AU-10' 'AU-16' 'CA-3'
+ 'CA-9' 'CM-14' 'CP-6' 'CP-9' 'CP-10' 'IA-2' 'IA-3' 'IA-4' 'IA-5' 'IA-6'
+ 'IA-7' 'IA-8' 'IA-9' 'IA-10' 'IA-11' 'IA-12' 'MA-5' 'MP-2' 'MP-3' 'MP-4'
+ 'MP-5' 'MP-7' 'PE-2' 'PE-3' 'PE-4' 'PE-5' 'PE-9' 'PE-17' 'PE-22' 'PM-12'
+ 'PS-2' 'PS-3' 'PS-4' 'PS-5' 'PS-6' 'PS-7' 'PT-8' 'SA-21' 'SC-8' 'SC-11'
+ 'SC-12' 'SC-13' 'SC-15' 'SC-16' 'SC-17' 'SC-20' 'SC-28' 'SC-36' 'SC-41'
+ 'SC-45' 'SC-46']</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>870</v>
+        <v>4830</v>
       </c>
       <c r="E3" t="n">
-        <v>124</v>
+        <v>558</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1425287356321839</v>
+        <v>0.115527950310559</v>
       </c>
       <c r="G3" t="n">
-        <v>7890</v>
+        <v>15610</v>
       </c>
       <c r="H3" t="n">
-        <v>203</v>
+        <v>343</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02572877059569075</v>
+        <v>0.02197309417040359</v>
       </c>
       <c r="J3" t="n">
-        <v>0.3792048929663608</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations, grouped by their general topic:
-**General Topic:** **System Access and Security Controls**
-*   **Access Control and Authentication:** The regulations focus heavily on controlling system access through various methods including limiting logon attempts, requiring alternative authentication factors, device locking, and authenticating devices before network connections are made.
-*   **User Notification and Awareness:** They emphasize the importance of user awareness through notifications of previous logon activity, account changes, and any additional information. There is also an emphasis on having users read and agree to rules of behavior.
-*   **Wireless and Mobile Device Security:**  These regulations cover how to securely use wireless technologies and how to enforce restrictions for mobile devices, especially when handling sensitive information, and to have controls on mobile device use outside controlled areas.
-*    **Data Protection and Auditing:** The regulations call for implementing measures to protect audit information, use non-repudiation to verify actions taken, monitor for information disclosure, protect transmitted data with cryptography, and manage cryptographic keys.
-*   **System Configuration and Integrity:** The regulations discuss the need to maintain baseline system configurations, using signed components, and controlling access to media, ports, and I/O devices. Also, rules of behavior and use of collaborative tools is covered.</t>
-        </is>
+        <v>0.6193118756936737</v>
       </c>
     </row>
     <row r="4">
@@ -2575,46 +2324,36 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CM-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1'
- 'PE-1' 'PL-1' 'PM-9' 'PS-1' 'PS-8' 'PT-1' 'RA-1' 'SA-1' 'SC-1' 'SC-38'
- 'SI-1' 'SI-12' 'SR-1']</t>
+          <t>['AC-22' 'AT-2' 'AT-3' 'AT-4' 'AU-13' 'CA-2' 'CA-5' 'CA-7' 'CP-3' 'CP-4'
+ 'IR-2' 'IR-3' 'PE-10' 'PE-14' 'PE-15' 'PL-4' 'PM-4' 'PM-6' 'PM-13'
+ 'PM-14' 'PM-15' 'PM-23' 'PM-25' 'PM-28' 'PM-31' 'PS-9' 'SA-11' 'SC-38'
+ 'SC-43' 'SI-20' 'SR-7']</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>506</v>
+        <v>930</v>
       </c>
       <c r="E4" t="n">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1600790513833992</v>
+        <v>0.1301075268817204</v>
       </c>
       <c r="G4" t="n">
-        <v>6210</v>
+        <v>8122</v>
       </c>
       <c r="H4" t="n">
-        <v>68</v>
+        <v>215</v>
       </c>
       <c r="I4" t="n">
-        <v>0.01095008051529791</v>
+        <v>0.0264713124846097</v>
       </c>
       <c r="J4" t="n">
-        <v>0.5436241610738255</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **Information Security and Privacy Management**.
-Here's a summary of the regulations:
-*   **Establish and Maintain Policies &amp; Procedures:** Organizations must develop, document, disseminate, and regularly review and update policies and procedures covering a wide range of security controls (e.g., access control, awareness, audit, incident response, etc.) and other topics (e.g., risk management, PII handling).
-*   **Designate Responsible Officials:** For each policy area, a designated official must manage the development, documentation, and dissemination of policies and procedures.
-*   **Implement Comprehensive Risk Management:** Organizations need to establish a strategy to manage security and privacy risks across their operations, implementing consistently across the organization, including supply chain.
-*   **Implement PII Protection:** Organizations must have policies for the processing and transparency of PII, limiting what elements they store and processes for research, testing, and training. Additionally, a process for disposal of PII.
-*  **Enforce Compliance &amp; Sanctions:** Organizations must have a process to enforce compliance, and sanction individuals who fail to comply with information security and privacy policies.</t>
-        </is>
+        <v>0.3601190476190476</v>
       </c>
     </row>
     <row r="5">
@@ -2622,48 +2361,35 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['AC-3' 'AC-16' 'AC-21' 'AT-2' 'AT-3' 'AT-4' 'CP-3' 'CP-4' 'IR-2' 'IR-3'
- 'IR-4' 'IR-6' 'IR-7' 'IR-8' 'IR-9' 'MP-3' 'MP-6' 'PE-10' 'PE-15' 'PE-22'
- 'PM-2' 'PM-5' 'PM-13' 'PM-14' 'PM-18' 'PM-19' 'PM-20' 'PM-21' 'PM-22'
- 'PM-23' 'PM-24' 'PM-26' 'PM-29' 'PS-9' 'PT-2' 'PT-3' 'PT-4' 'PT-5' 'PT-6'
- 'PT-7' 'PT-8' 'RA-8' 'SC-42' 'SI-18' 'SI-19' 'SR-12']</t>
+          <t>['AC-21' 'AC-23' 'IR-6' 'IR-7' 'IR-8' 'IR-9' 'MP-6' 'PM-2' 'PM-5' 'PM-18'
+ 'PM-19' 'PM-20' 'PM-21' 'PM-22' 'PM-24' 'PM-26' 'PM-29' 'PT-1' 'PT-2'
+ 'PT-3' 'PT-4' 'PT-5' 'PT-6' 'PT-7' 'SC-42' 'SI-18' 'SI-19' 'SR-12']</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2070</v>
+        <v>756</v>
       </c>
       <c r="E5" t="n">
-        <v>244</v>
+        <v>100</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1178743961352657</v>
+        <v>0.1322751322751323</v>
       </c>
       <c r="G5" t="n">
-        <v>11362</v>
+        <v>7420</v>
       </c>
       <c r="H5" t="n">
-        <v>217</v>
+        <v>105</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01909875022003168</v>
+        <v>0.01415094339622642</v>
       </c>
       <c r="J5" t="n">
-        <v>0.5292841648590022</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations, broken down into concise bullet points, along with the general topic:
-**General Topic:** Cybersecurity and Privacy Controls
-*   **Access Control and Data Protection:** The regulations emphasize strict enforcement of access controls, including mandatory, discretionary, role-based, and attribute-based access, along with the protection of security-relevant information. It also highlights the need for dual authorization for sensitive operations and controlled release of information.
-*   **Security and Privacy Attributes:** There is a heavy focus on the association, maintenance, and consistent interpretation of security and privacy attributes with information throughout its lifecycle, including requirements for dynamic attribute association and controlled modification.
-*   **Training and Awareness:** The regulations mandate comprehensive security and privacy literacy training for all users, with role-based training for specific personnel, covering various topics such as insider threats, social engineering, incident response, and contingency planning, along with requirements for training records.
-*  **Incident Response and Handling:** A significant portion of the regulations pertains to incident response, from initial training to testing and the actual handling of security incidents, as well as the establishment of security operations center, and public relation handling of incidents. This includes spill response and media sanitization and disposal.
-*   **Privacy Program and Data Governance:** The rules also emphasize the development and implementation of a privacy program, data governance practices, as well as the need for policies and procedures relating to personally identifiable information, including authority to process, data quality, transparency, consent, and de-identification.</t>
-        </is>
+        <v>0.4878048780487805</v>
       </c>
     </row>
     <row r="6">
@@ -2671,50 +2397,37 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['AC-2' 'AC-5' 'AC-6' 'AC-8' 'AC-10' 'AC-12' 'AC-14' 'AC-17' 'AC-20'
- 'AC-23' 'AU-2' 'AU-3' 'AU-4' 'AU-5' 'AU-6' 'AU-7' 'AU-8' 'AU-11' 'AU-12'
- 'AU-14' 'AU-16' 'CA-3' 'IA-2' 'IA-4' 'IA-5' 'IA-6' 'IA-8' 'IA-10' 'IA-11'
- 'IA-12' 'IR-5' 'MA-4' 'MA-5' 'MA-7' 'PE-2' 'PE-3' 'PE-5' 'PE-6' 'PE-8'
- 'PM-12' 'PS-2' 'PS-3' 'PS-4' 'PS-5' 'PS-6' 'PS-7' 'SA-21' 'SC-10' 'SC-11'
- 'SC-23' 'SC-45' 'SC-48' 'SI-14' 'SI-21']</t>
+          <t>['AC-25' 'CA-6' 'CM-12' 'CM-13' 'MA-6' 'PL-2' 'PL-7' 'PL-8' 'PL-10'
+ 'PL-11' 'PM-1' 'PM-3' 'PM-7' 'PM-10' 'PM-11' 'PM-17' 'PM-27' 'PM-32'
+ 'RA-2' 'RA-3' 'RA-6' 'RA-7' 'RA-8' 'RA-9' 'RA-10' 'SA-2' 'SA-3' 'SA-4'
+ 'SA-5' 'SA-8' 'SA-9' 'SA-16' 'SA-17' 'SA-22' 'SA-23' 'SC-2' 'SC-3' 'SC-4'
+ 'SC-32' 'SC-39' 'SC-49' 'SC-50' 'SI-16' 'SR-2']</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2862</v>
+        <v>1892</v>
       </c>
       <c r="E6" t="n">
-        <v>358</v>
+        <v>218</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1250873515024458</v>
+        <v>0.1152219873150106</v>
       </c>
       <c r="G6" t="n">
-        <v>12906</v>
+        <v>10956</v>
       </c>
       <c r="H6" t="n">
-        <v>293</v>
+        <v>259</v>
       </c>
       <c r="I6" t="n">
-        <v>0.02270261893692856</v>
+        <v>0.02364001460387002</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5499231950844854</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulations, focusing on the core topics:
-**General Topic: Access Control, Authentication, and Audit Logging**
-*   **Account and User Management:**  Regulations emphasize the complete lifecycle management of user accounts, from creation and authorization, to disabling, monitoring, and handling termination of accounts, as well as requirements for shared accounts, and dynamic privilege management.
-*   **Authentication and Identification:**  Multi-factor authentication (MFA) is a common requirement for both privileged and non-privileged accounts along with the use of Personal Identity Verification (PIV) credentials. This includes strong password policies and replay-resistant authentication measures, as well as management of user identifiers and authenticators.
-*   **Remote Access and External Systems:** Regulations mandate controls for remote access including monitoring, encryption, routing through authorized points, and protection of remote access mechanisms. There are also restrictions on use of external and personal systems for organizational information.
-*   **Session Management:** Rules are included for controlling concurrent sessions, automatically terminating sessions after inactivity or specific events, and providing clear messages for user logouts, along with protection of session authenticity, and system time synchronization. 
-*   **Audit Logging and Monitoring:** Comprehensive requirements for audit logging, including event types, content of records, storage capacity, and response to failures are set.  These logs must be analyzed and correlated, and include reporting features for investigations. Physical access monitoring is also included.
-*   **Personnel Security and Access:** Rules for screening, background checks, and termination of personnel are covered, along with access agreements and the insider threat program. Also includes access to facilities based on roles.</t>
-        </is>
+        <v>0.4570230607966457</v>
       </c>
     </row>
     <row r="7">
@@ -2722,46 +2435,35 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['CP-2' 'CP-6' 'CP-7' 'CP-8' 'CP-9' 'CP-10' 'CP-11' 'CP-12' 'CP-13'
- 'PE-11' 'PE-12' 'PE-13' 'PE-18' 'PE-19' 'PE-20' 'PE-21' 'PE-23' 'PM-8'
- 'SC-4' 'SC-6' 'SC-7' 'SC-20' 'SC-21' 'SC-22' 'SC-24' 'SC-36' 'SC-47'
- 'SI-13' 'SI-17']</t>
+          <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CM-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1'
+ 'PE-1' 'PL-1' 'PM-9' 'PS-1' 'PS-8' 'RA-1' 'SA-1' 'SC-1' 'SI-1' 'SI-12'
+ 'SR-1']</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>812</v>
+        <v>420</v>
       </c>
       <c r="E7" t="n">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1366995073891626</v>
+        <v>0.1809523809523809</v>
       </c>
       <c r="G7" t="n">
-        <v>7656</v>
+        <v>5712</v>
       </c>
       <c r="H7" t="n">
-        <v>134</v>
+        <v>62</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01750261233019854</v>
+        <v>0.01085434173669468</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4530612244897959</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>**General Topic:** System and Network Resiliency, Business Continuity, and Disaster Recovery
-*   **Contingency Planning and Alternate Sites:** Organizations must have comprehensive contingency plans, establish alternate processing and storage sites, and secure backup systems to maintain essential functions during disruptions.
-*   **Telecommunications and Power Redundancy:** Alternate telecommunications services and emergency power supplies must be in place to ensure continued operations, along with fire suppression systems to protect the facilities.
-*   **Boundary Protection and Network Security:** Implement robust boundary protection measures with managed interfaces, segmentation of networks, and prevent data exfiltration to safeguard the system from internal and external threats.
-*   **Secure Name Resolution and System Stability:** Ensure secure and reliable name/address resolution services and implement fail-safe procedures to maintain operational integrity during system failures.
-*   **Distributed Systems and Failure Prevention:** Distribute critical system components across multiple locations, use polling techniques to identify faults, and implement procedures to transfer component responsibilities to prevent predictable failures.</t>
-        </is>
+        <v>0.5507246376811594</v>
       </c>
     </row>
     <row r="8">
@@ -2769,50 +2471,36 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['CA-2' 'CA-5' 'CA-6' 'CA-7' 'CA-8' 'CM-4' 'CM-7' 'MA-2' 'MA-3' 'MA-6'
- 'PE-14' 'PE-16' 'PL-2' 'PL-7' 'PL-8' 'PL-10' 'PL-11' 'PM-1' 'PM-3' 'PM-4'
- 'PM-6' 'PM-7' 'PM-10' 'PM-11' 'PM-15' 'PM-17' 'PM-25' 'PM-28' 'PM-30'
- 'PM-31' 'PM-32' 'RA-2' 'RA-3' 'RA-5' 'RA-6' 'RA-7' 'RA-9' 'RA-10' 'SA-2'
- 'SA-3' 'SA-4' 'SA-5' 'SA-8' 'SA-9' 'SA-10' 'SA-11' 'SA-15' 'SA-16'
- 'SA-17' 'SA-20' 'SA-22' 'SA-23' 'SC-2' 'SC-3' 'SC-25' 'SC-27' 'SC-29'
- 'SC-30' 'SC-32' 'SC-50' 'SI-2' 'SI-5' 'SI-6' 'SR-2' 'SR-3' 'SR-4' 'SR-5'
- 'SR-6' 'SR-7' 'SR-8' 'SR-9' 'SR-10' 'SR-11']</t>
+          <t>['AC-10' 'AC-12' 'CA-8' 'CP-2' 'CP-7' 'CP-8' 'CP-11' 'CP-12' 'CP-13'
+ 'PE-11' 'PE-12' 'PE-13' 'PE-18' 'PE-19' 'PE-20' 'PE-21' 'PE-23' 'PM-8'
+ 'SA-20' 'SC-6' 'SC-7' 'SC-10' 'SC-21' 'SC-22' 'SC-23' 'SC-24' 'SC-40'
+ 'SC-47' 'SC-48' 'SI-13' 'SI-14' 'SI-17' 'SI-21']</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5256</v>
+        <v>1056</v>
       </c>
       <c r="E8" t="n">
-        <v>531</v>
+        <v>86</v>
       </c>
       <c r="F8" t="n">
-        <v>0.101027397260274</v>
+        <v>0.08143939393939394</v>
       </c>
       <c r="G8" t="n">
-        <v>16060</v>
+        <v>8580</v>
       </c>
       <c r="H8" t="n">
-        <v>346</v>
+        <v>133</v>
       </c>
       <c r="I8" t="n">
-        <v>0.02154420921544209</v>
+        <v>0.0155011655011655</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6054732041049031</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>**General Topic:** System and Information Security Management
-*   **Comprehensive Security Lifecycle:** These regulations cover the entire lifecycle of a system, from initial planning and design through development, acquisition, maintenance, and disposal.
-*   **Risk Management Focus:** A strong emphasis on risk assessment, monitoring, and response to vulnerabilities, threats, and supply chain risks.
-*   **Continuous Monitoring &amp; Improvement:**  Requires ongoing assessments, vulnerability scans, and penetration testing to ensure the effectiveness of security controls and to drive continuous improvement.
-*   **System and Component Integrity:**  Focus on ensuring the integrity of both software and hardware through rigorous configuration management, testing, and development practices.
-*   **Supply Chain Security:** Strong requirements for supply chain risk management with focus on supplier vetting, provenance tracking, and tamper protection.</t>
-        </is>
+        <v>0.3926940639269406</v>
       </c>
     </row>
   </sheetData>
@@ -2826,7 +2514,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -2888,56 +2576,39 @@
           <t>inner connections probability</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['CM-2' 'CM-3' 'CM-4' 'CM-5' 'CM-6' 'CM-7' 'CM-8' 'CM-9' 'CM-10' 'CM-11'
- 'MA-2' 'RA-5' 'SA-10' 'SC-37' 'SI-2' 'SI-6' 'SI-7' 'SI-10' 'SR-4' 'SR-11']</t>
+          <t>['AT-3' 'PE-1' 'PE-4' 'PE-9' 'PE-10' 'PE-13' 'PE-14' 'PE-15' 'PS-9']</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>380</v>
+        <v>72</v>
       </c>
       <c r="E2" t="n">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3815789473684211</v>
+        <v>0.2083333333333333</v>
       </c>
       <c r="G2" t="n">
-        <v>5460</v>
+        <v>2556</v>
       </c>
       <c r="H2" t="n">
-        <v>216</v>
+        <v>40</v>
       </c>
       <c r="I2" t="n">
-        <v>0.03956043956043956</v>
+        <v>0.01564945226917058</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4016620498614958</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>The general topic of these cyber regulations is **System and Information Integrity**.
-Here's a summary of the regulations:
-*   **Baseline and Change Management:** The regulations emphasize creating and maintaining secure baseline configurations for systems, controlling changes, and analyzing the potential impacts of those changes. Automated tools for change management, documentation, and approval processes are recommended.
-*   **Access Control &amp; Least Functionality:** Access restrictions for system changes are mandated, with the requirement for dual authorization for critical components. The principle of least functionality is stressed, urging systems to only include necessary capabilities and restrict unnecessary software, services, and ports.
-*   **System Component Inventory &amp; Integrity:** Comprehensive inventory management of system components is crucial, including tracking, location, accountability, and automated unauthorized component detection. Integrity checks, especially for software, firmware, and the boot process, are also mandated.
-*    **Vulnerability Management and Remediation:** The regulations require regular vulnerability monitoring and scanning, along with the timely remediation of identified flaws. Automated tools are encouraged, and information sharing on vulnerabilities is deemed important for eliminating them across systems. 
-*   **Software and Supply Chain Integrity:** The regulations address software usage restrictions, with special attention to user-installed software and open-source components. Provenance is important in supply chain management, and the detection and prevention of counterfeit components are also essential.</t>
-        </is>
+        <v>0.2727272727272727</v>
       </c>
     </row>
     <row r="3">
@@ -2945,45 +2616,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['AT-2' 'AT-3' 'IR-2' 'IR-8' 'IR-9' 'PE-10' 'PE-15' 'PM-13' 'PM-20'
- 'PM-21' 'PS-9' 'PT-1' 'PT-2' 'PT-3' 'PT-4' 'PT-5' 'PT-6' 'PT-7' 'SA-16'
- 'SC-42']</t>
+          <t>['AC-4' 'AC-6' 'AU-2' 'AU-3' 'AU-7' 'AU-8' 'AU-12' 'PM-24' 'PT-8' 'SA-17'
+ 'SC-31' 'SC-45' 'SC-46' 'SI-10' 'SI-11']</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>380</v>
+        <v>210</v>
       </c>
       <c r="E3" t="n">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2078947368421053</v>
+        <v>0.2380952380952381</v>
       </c>
       <c r="G3" t="n">
-        <v>5460</v>
+        <v>4170</v>
       </c>
       <c r="H3" t="n">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="I3" t="n">
-        <v>0.0206959706959707</v>
+        <v>0.03213429256594724</v>
       </c>
       <c r="J3" t="n">
-        <v>0.4114583333333333</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>**General Topic:** Cybersecurity and Privacy Training, Incident Response, and Data Protection
-*   **Mandatory Training:** Organizations must provide comprehensive security and privacy training to all personnel, including literacy training, role-based training, incident response training, and information spillage training. Training should be initial, recurring, and updated for changes.
-*   **Incident Response:** Organizations are required to develop and maintain a detailed incident response plan, implement incident response training that includes simulated exercises, and establish automated training environments for incident response. Special consideration is given to data breaches involving PII.
-*   **PII Protection:** Organizations must establish policies and procedures for processing personally identifiable information (PII), document their authority and purpose for processing PII, and implement mechanisms for consent and privacy notices. Specific rules apply to special PII categories (like SSNs).
-*   **Transparency and Accountability:** Organizations must make privacy policies publicly available, maintain records of disclosures of PII, and provide a way for the public to communicate with privacy offices.
-*   **Physical Security and Operational Safeguards:** Organizations must implement physical safeguards such as emergency shutoff procedures and water damage protection mechanisms, and also address the use of sensors, data collection, and personnel roles.</t>
-        </is>
+        <v>0.2717391304347826</v>
       </c>
     </row>
     <row r="4">
@@ -2991,45 +2651,34 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['AC-10' 'AC-12' 'AC-17' 'MA-4' 'MA-7' 'MP-6' 'SC-8' 'SC-10' 'SC-23'
- 'SR-12']</t>
+          <t>['CP-2' 'CP-6' 'CP-7' 'CP-8' 'CP-9' 'CP-10' 'CP-11' 'MP-2' 'MP-4' 'MP-5'
+ 'PE-11' 'PE-12' 'SC-36' 'SC-47']</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
+        <v>182</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>67</v>
       </c>
       <c r="F4" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.3681318681318682</v>
       </c>
       <c r="G4" t="n">
-        <v>2830</v>
+        <v>3906</v>
       </c>
       <c r="H4" t="n">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="I4" t="n">
-        <v>0.02720848056537102</v>
+        <v>0.02534562211981567</v>
       </c>
       <c r="J4" t="n">
-        <v>0.2376237623762376</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **Session Management, Remote Access, Data Handling, and Transmission Security**.
-Here is a summary of the regulations in bullet points:
-*   **Session Control &amp; Termination:**  Regulations focus on limiting concurrent sessions, automatically terminating inactive sessions, providing user logout options with confirmation messages, and warning users of impending timeouts.
-*   **Remote Access Security:** These regulations require documentation, authorization, monitoring, and strong encryption of remote access sessions, including authentication of commands, and protection of mechanism information, alongside the capability to disable remote access quickly.
-*  **Maintenance &amp; Disposal Safeguards**: Rules mandate secure, authorized non-local maintenance practices, including authentication, separation from regular sessions, and proper logging. Disposal also requires media sanitization, verification, and destruction of data and components.
-*   **Transmission Protection:** Regulations necessitate securing the confidentiality and integrity of transmitted information using cryptography, addressing pre- and post-transmission handling, protecting message externals, and concealing/randomizing communication patterns.
-*   **Session Authenticity &amp; Network Control:** Rules require verifying session authenticity using unique identifiers, invalidating identifiers upon logout, and controlling the use of authorized certificate authorities.  They also mandate termination of network connections at the end of sessions or after periods of inactivity.</t>
-        </is>
+        <v>0.4036144578313253</v>
       </c>
     </row>
     <row r="5">
@@ -3037,44 +2686,35 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['CP-3' 'CP-4' 'CP-8' 'CP-11' 'CP-12' 'CP-13' 'IR-3' 'SC-24' 'SC-47'
- 'SI-17']</t>
+          <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1' 'PL-1'
+ 'PM-2' 'PM-9' 'PM-18' 'PM-19' 'PM-29' 'PS-1' 'PS-8' 'RA-1' 'SA-1' 'SI-12'
+ 'SR-1']</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>90</v>
+        <v>420</v>
       </c>
       <c r="E5" t="n">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2444444444444444</v>
+        <v>0.1595238095238095</v>
       </c>
       <c r="G5" t="n">
-        <v>2830</v>
+        <v>5712</v>
       </c>
       <c r="H5" t="n">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="I5" t="n">
-        <v>0.01413427561837456</v>
+        <v>0.01137955182072829</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3548387096774194</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>**General Topic:** Business Continuity and Disaster Recovery
-*   **Contingency Training:** Requires regular, role-based training for system users, incorporating simulations and realistic environments.
-*   **Contingency Plan Testing:** Mandates regular testing of the contingency plan, including at alternate sites, with full recovery procedures, and coordination with related plans.
-*  **Telecommunications Services:** Requires establishing alternate telecommunications with priority agreements, diverse providers, provider contingency plans, and regular testing.
-*   **Incident Response Testing:** Dictates regular testing of incident response capabilities, using automation, coordination with related plans, and continuous improvement based on test data.
-*   **System Resilience:** Focuses on maintaining system operations through safe mode, alternate security mechanisms, known fail states, alternate communication paths, and fail-safe procedures in case of disruptions.</t>
-        </is>
+        <v>0.5075757575757576</v>
       </c>
     </row>
     <row r="6">
@@ -3082,46 +2722,34 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CM-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1'
- 'PE-1' 'PL-1' 'PM-2' 'PM-9' 'PS-1' 'PS-8' 'RA-1' 'SA-1' 'SC-1' 'SI-1'
- 'SI-12']</t>
+          <t>['CM-2' 'CM-3' 'CM-4' 'CM-5' 'CM-6' 'CM-7' 'CM-8' 'CM-9' 'CM-10' 'CM-11'
+ 'CM-14' 'MA-2' 'PL-9' 'SC-28' 'SC-34' 'SC-37' 'SI-2' 'SI-7']</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>420</v>
+        <v>306</v>
       </c>
       <c r="E6" t="n">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1738095238095238</v>
+        <v>0.369281045751634</v>
       </c>
       <c r="G6" t="n">
-        <v>5712</v>
+        <v>4950</v>
       </c>
       <c r="H6" t="n">
-        <v>61</v>
+        <v>209</v>
       </c>
       <c r="I6" t="n">
-        <v>0.01067927170868347</v>
+        <v>0.04222222222222222</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5447761194029851</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **Comprehensive Information Security and Privacy Management**.
-Here's a summary:
-*   **Policy and Procedure Development:**  Organizations must develop, document, disseminate, and regularly review policies and procedures for various security and privacy controls. These policies must cover purpose, scope, roles, responsibilities, management commitment, coordination and compliance with relevant laws and regulations.
-*   **Designated Management:**  A designated official is required to manage the development, documentation, and dissemination of each policy and its associated procedures.
-*   **Specific Control Areas:** The regulations require policies and procedures for: access control, awareness &amp; training, audit &amp; accountability, assessment, authorization, and monitoring, configuration management, contingency planning, identification &amp; authentication, incident response, maintenance, media protection, physical &amp; environmental protection, planning, personnel security, risk assessment, system &amp; service acquisition, system &amp; communications protection, system &amp; information integrity.
-*   **Risk Management and Leadership:**  Organizations must have a senior information security officer to lead an organization-wide security program and implement a comprehensive risk management strategy, which includes privacy risks.
-*   **Personnel Accountability:** Formal sanctions must be in place for individuals who fail to comply with security and privacy policies, along with a process to notify relevant personnel when these sanctions are initiated. Additionally, information management must adhere to applicable laws, regulations, and operational needs, with a specific focus on limiting and protecting personally identifiable information.</t>
-        </is>
+        <v>0.3509316770186335</v>
       </c>
     </row>
     <row r="7">
@@ -3129,44 +2757,34 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['AC-21' 'CA-2' 'CA-3' 'CA-6' 'PE-18' 'PE-19' 'PE-20' 'PE-21' 'PE-23'
- 'PM-8' 'PM-17' 'RA-3' 'RA-6' 'RA-10' 'SC-15' 'SC-38']</t>
+          <t>['CM-1' 'SA-8' 'SA-20' 'SA-23' 'SC-1' 'SC-2' 'SC-4' 'SC-32' 'SC-49'
+ 'SC-50' 'SI-1']</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>240</v>
+        <v>110</v>
       </c>
       <c r="E7" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1541666666666667</v>
+        <v>0.1909090909090909</v>
       </c>
       <c r="G7" t="n">
-        <v>4432</v>
+        <v>3102</v>
       </c>
       <c r="H7" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="I7" t="n">
-        <v>0.02030685920577617</v>
+        <v>0.02675693101225016</v>
       </c>
       <c r="J7" t="n">
-        <v>0.2913385826771653</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>**General Topic:** System Security and Risk Management
-*   **Information Sharing and Exchange:** Regulations focus on controlled sharing of information, use of automated decision support, enforcing sharing restrictions, and formalizing information exchange agreements between systems.
-*   **Control Assessments:**  Establish a framework for assessing the effectiveness of security controls through planning, independent assessments, and specialized techniques, while also leveraging external assessments where appropriate.
-*   **System Authorization:** Requires formal authorization processes involving senior officials, both internally and across organizations, before system operations begin and for ongoing use.
-*   **Physical Security and Environmental Protection:** Includes measures for physical placement of system components, protection from electromagnetic leakage, asset monitoring, and addressing environmental hazards.
-*   **Risk Management and Threat Awareness:** Requires comprehensive risk assessments, including supply chain, all-source intelligence, and dynamic threat awareness with predictive analytics to identify, mitigate, and respond to risks to the systems and organization.</t>
-        </is>
+        <v>0.2019230769230769</v>
       </c>
     </row>
     <row r="8">
@@ -3174,45 +2792,33 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['AC-4' 'AC-16' 'AU-10' 'CM-14' 'IA-7' 'MP-3' 'PE-22' 'SC-11' 'SC-12'
- 'SC-13' 'SC-16' 'SC-17' 'SC-20' 'SC-46' 'SC-49' 'SC-50']</t>
+          <t>['IR-4' 'IR-5' 'IR-6' 'IR-7' 'IR-8' 'PE-6' 'PE-8' 'PT-1' 'SR-8']</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>240</v>
+        <v>72</v>
       </c>
       <c r="E8" t="n">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="F8" t="n">
-        <v>0.2208333333333333</v>
+        <v>0.3888888888888889</v>
       </c>
       <c r="G8" t="n">
-        <v>4432</v>
+        <v>2556</v>
       </c>
       <c r="H8" t="n">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="I8" t="n">
-        <v>0.02346570397111913</v>
+        <v>0.02582159624413146</v>
       </c>
       <c r="J8" t="n">
-        <v>0.3375796178343949</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **Information Flow Control and Security Attribute Management**.
-Here's a summary of the key points:
-*   **Enforce Information Flow Policies:** The regulations heavily emphasize enforcing organization-defined policies to control the flow of information within and between systems, using various methods like protected processing domains, metadata, and one-way mechanisms. They also include specific requirements for encrypted information and data types.
-*   **Security and Privacy Attributes:**  A significant portion of the regulations focuses on the association, maintenance, and transmission of security and privacy attributes with information. This includes dynamic association, authorized changes, consistent interpretation, and attribute display on output devices.
-*   **Cross-Domain Security:** Many regulations address secure information transfer between different security domains. This includes the use of filters, sanitization, unique identification, metadata validation, and the separation of information flows, both physically and logically.
-*   **Non-Repudiation &amp; Trusted Systems:**  The regulations require irrefutable evidence of actions, binding identities to information, and maintaining chains of custody. They also include requirements for trusted paths for communication between users and trusted system components.
-*   **Cryptographic Controls and Key Management:** The regulations specify how cryptographic keys are managed (generation, distribution, storage, destruction) and used within the system. They also cover digital signing of components and the implementation of cryptographic module authentication, including public key infrastructure certificates.</t>
-        </is>
+        <v>0.2978723404255319</v>
       </c>
     </row>
     <row r="9">
@@ -3220,45 +2826,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['AU-2' 'AU-3' 'AU-4' 'AU-5' 'AU-6' 'AU-7' 'AU-8' 'AU-9' 'AU-11' 'AU-12'
- 'AU-14' 'AU-16' 'IR-5' 'PE-6' 'SC-5' 'SC-31' 'SC-40' 'SC-48' 'SI-4'
- 'SI-11']</t>
+          <t>['AU-13' 'CA-2' 'CA-5' 'CA-6' 'CA-7' 'CA-8' 'PM-3' 'PM-4' 'PM-6' 'PM-10'
+ 'PM-23' 'PM-28' 'PM-31' 'RA-5' 'RA-6' 'RA-7' 'RA-10' 'SC-38' 'SI-20']</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="E9" t="n">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3105263157894737</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="G9" t="n">
-        <v>5460</v>
+        <v>5206</v>
       </c>
       <c r="H9" t="n">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="I9" t="n">
-        <v>0.03113553113553114</v>
+        <v>0.02804456396465617</v>
       </c>
       <c r="J9" t="n">
-        <v>0.4097222222222222</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>**General Topic:** System and Information Integrity (specifically focusing on audit logging, system monitoring, and denial-of-service protection)
-*   **Comprehensive Audit Logging:** These regulations mandate detailed audit logging, including what events to log, the content of audit records (what, when, where, source, outcome, identity), storage capacity, and how to handle failures in logging processes.
-*  **Proactive System Monitoring:**  The regulations emphasize continuous system monitoring to detect attacks, unauthorized connections, and unusual activities. This includes real-time analysis, integrating monitoring tools, and analysis of both inbound/outbound communications traffic. 
-*   **Incident Response and Analysis:**  There are regulations around reviewing and analyzing audit records and system monitoring data. This involves reporting findings, integrating automated processes, and correlating information to build awareness. Incident tracking and analysis is also a required part of the organization's security posture. 
-* **Physical and Wireless Security:**  The regulations cover physical security measures, such as monitoring physical access, as well as wireless security through the protection of wireless links and intrusion detection systems.
-*   **Denial-of-Service &amp; Covert Channel Mitigation:** Regulations require protection against denial-of-service attacks and analysis and mitigation of covert communication channels within the system.</t>
-        </is>
+        <v>0.3302752293577982</v>
       </c>
     </row>
     <row r="10">
@@ -3266,45 +2861,34 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['AT-4' 'AU-13' 'CA-5' 'CA-7' 'PE-14' 'PM-3' 'PM-4' 'PM-6' 'PM-14' 'PM-15'
- 'PM-28' 'PM-31' 'RA-7' 'SI-5' 'SI-20']</t>
+          <t>['AC-22' 'AT-2' 'AT-4' 'CP-3' 'CP-4' 'IR-2' 'IR-3' 'IR-9' 'PM-12' 'PM-13'
+ 'PM-14' 'PM-16']</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>210</v>
+        <v>132</v>
       </c>
       <c r="E10" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1904761904761905</v>
+        <v>0.3257575757575757</v>
       </c>
       <c r="G10" t="n">
-        <v>4170</v>
+        <v>3372</v>
       </c>
       <c r="H10" t="n">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02757793764988009</v>
+        <v>0.02164887307236062</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2580645161290323</v>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **Continuous Monitoring and Risk Management for Cybersecurity and Privacy**.
-Here's a summary of the regulations in concise bullet points:
-*   **Establish Continuous Monitoring Programs:** Implement system-wide and organization-wide continuous monitoring strategies, including defined metrics, assessment frequencies, and reporting mechanisms; utilize independent assessments, trend analyses, risk monitoring, and consistency analysis.
-*   **Develop and Maintain Remediation Plans:** Create and update Plans of Action and Milestones (POA&amp;Ms) for documented weaknesses, utilizing automation for accuracy; implement a process for ensuring these plans address risks to organizational operations, assets, individuals, other organizations, and the Nation.
-*   **Monitor for Threats and Vulnerabilities:** Actively monitor for information disclosures, unauthorized replication of data, and environmental conditions that could affect systems; establish contact with security and privacy groups and associations to stay up to date on emerging threats.
-*  **Implement Security and Privacy Policies:** Document training activities, monitor performance metrics, and make available necessary resources to implement information security and privacy programs.
-*   **Manage and Respond to Risk:** Define risk tolerances, respond to security assessments and audits, disseminate and implement security alerts and advisories, and use tainting to identify data exfiltration; implement risk response actions.</t>
-        </is>
+        <v>0.3706896551724138</v>
       </c>
     </row>
     <row r="11">
@@ -3312,44 +2896,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['CA-8' 'MP-2' 'MP-4' 'PE-3' 'PE-4' 'PE-5' 'PE-8' 'PE-9' 'SC-28' 'SC-34']</t>
+          <t>['PE-16' 'PM-30' 'SA-4' 'SA-5' 'SA-10' 'SA-16' 'SC-25' 'SC-27' 'SC-29'
+ 'SC-30' 'SR-3' 'SR-5' 'SR-6' 'SR-9' 'SR-10' 'SR-11']</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>90</v>
+        <v>240</v>
       </c>
       <c r="E11" t="n">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3222222222222222</v>
+        <v>0.2666666666666667</v>
       </c>
       <c r="G11" t="n">
-        <v>2830</v>
+        <v>4432</v>
       </c>
       <c r="H11" t="n">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="I11" t="n">
-        <v>0.03321554770318021</v>
+        <v>0.02594765342960289</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2357723577235772</v>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **Physical and Environmental Security Controls**.
-Here's a summary of the regulations in concise bullet points:
-*   **Penetration Testing:** Regularly conduct both internal and external penetration testing, including physical facility testing, using independent teams and red team exercises.
-*   **Media Protection:** Implement strict access control, secure storage, and sanitization procedures for all digital and non-digital media.
-*   **Physical Access Control:** Enforce physical access authorizations, maintain logs, control visitor access, secure physical access devices, and implement physical barriers. This includes measures for system components and transmission lines.
-*   **Physical Security Measures:** Protect power equipment and cabling from damage, implement redundant cabling, employ anti-tamper technologies, and ensure secure access to output devices.
-*   **Data Protection:** Implement measures to protect information at rest, including encryption, secure storage, and read-only media for executables, as well as maintain visitor access records.</t>
-        </is>
+        <v>0.3575418994413408</v>
       </c>
     </row>
     <row r="12">
@@ -3357,45 +2931,34 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['CP-2' 'CP-6' 'CP-7' 'CP-9' 'CP-10' 'MA-6' 'MP-5' 'PE-11' 'PE-12' 'PE-13'
- 'SC-6' 'SC-36' 'SI-13']</t>
+          <t>['AC-16' 'AC-21' 'AC-23' 'MP-3' 'PE-22' 'PM-27' 'PT-4' 'SC-11' 'SC-15'
+ 'SC-42']</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="E12" t="n">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3525641025641026</v>
+        <v>0.1888888888888889</v>
       </c>
       <c r="G12" t="n">
-        <v>3640</v>
+        <v>2830</v>
       </c>
       <c r="H12" t="n">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0239010989010989</v>
+        <v>0.01307420494699647</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3873239436619718</v>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>The general topic for all of these regulations is **System and Information Availability and Business Continuity**.
-Here's a summary of the regulations in bullet points:
-*   **Comprehensive Contingency Planning:** Organizations must develop, maintain, and regularly review a detailed contingency plan that includes roles, responsibilities, recovery objectives, and coordination with other plans and external providers.
-*   **Alternate Processing and Storage:** Establish and maintain alternate processing and storage sites that are separated from primary sites, ensuring they have equivalent controls, are accessible, and can meet recovery time objectives.
-*   **System Backup and Recovery:** Implement regular backups of user, system, and documentation data, testing their reliability and integrity, and storing critical backups separately. Ensure systems can be recovered and reconstituted to a known state within defined timeframes.
-*   **Maintenance and Resource Management:** Provide timely maintenance (including preventive and predictive) for system components, ensure the availability of spare parts, and allocate resources based on defined priorities and controls.
-*   **Infrastructure Protection and Resilience:** Implement measures to ensure system availability, including uninterruptible and alternate power supplies, emergency lighting, fire protection systems with automatic activation, and mechanisms to prevent failures, with distributed processing and failover capabilities.</t>
-        </is>
+        <v>0.3148148148148148</v>
       </c>
     </row>
     <row r="13">
@@ -3403,45 +2966,35 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['IA-3' 'IA-4' 'IA-5' 'IA-6' 'IA-9' 'IA-12' 'PE-2' 'PM-12' 'PS-2' 'PS-3'
- 'PS-4' 'PS-5' 'PS-6' 'PS-7' 'SA-21']</t>
+          <t>['AC-7' 'AC-9' 'AC-10' 'AC-11' 'AC-12' 'AC-17' 'AC-18' 'AC-19' 'CA-9'
+ 'IA-3' 'IA-7' 'MA-4' 'MA-7' 'PE-17' 'PL-4' 'SC-8' 'SC-10' 'SC-12' 'SC-13'
+ 'SC-23' 'SC-40']</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>210</v>
+        <v>420</v>
       </c>
       <c r="E13" t="n">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.2357142857142857</v>
       </c>
       <c r="G13" t="n">
-        <v>4170</v>
+        <v>5712</v>
       </c>
       <c r="H13" t="n">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="I13" t="n">
-        <v>0.02398081534772182</v>
+        <v>0.0274859943977591</v>
       </c>
       <c r="J13" t="n">
-        <v>0.4350282485875706</v>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>The general topic for these regulations is **Identity and Access Management**.
-Here's a summary of the regulations:
-*   **Device &amp; Service Authentication:** Devices and services must be uniquely identified and authenticated using strong cryptographic methods before establishing connections. Dynamic IP address allocation and device attestation are key.
-*   **Identifier Management:**  System identifiers must be managed, assigned, and protected with controls to prevent reuse and unauthorized access. They should also be uniquely managed for individuals and attributes maintained in a secure central storage.
-*   **Authenticator Management:** System authenticators (passwords, keys, biometrics) must be managed securely. This includes strong creation, storage, and management procedures to prevent compromise and unauthorized access and should be changed regularly. Use of GSA-approved products and services is required.
-*   **Identity Proofing:** Identity proofing procedures are needed to ensure that individuals are who they claim to be prior to receiving system access and that identities are validated by a registration authority, and address confirmation for the user.
-*   **Personnel Security:**  Personnel security is crucial, with requirements for physical access authorization, insider threat programs, position risk designations, screening, and proper procedures for termination, transfer, access agreements, and external personnel security as well as developer screening.</t>
-        </is>
+        <v>0.38671875</v>
       </c>
     </row>
     <row r="14">
@@ -3449,43 +3002,34 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['PE-16' 'PM-1' 'PM-18' 'PM-30' 'SR-1' 'SR-2' 'SR-6' 'SR-7' 'SR-10']</t>
+          <t>['AC-2' 'MA-5' 'PE-2' 'PE-3' 'PE-5' 'PE-18' 'PE-19' 'PE-20' 'PE-21'
+ 'PE-23' 'PM-8' 'PS-2' 'PS-3' 'PS-4' 'PS-5' 'PS-6' 'PS-7' 'SA-21']</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>72</v>
+        <v>306</v>
       </c>
       <c r="E14" t="n">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1805555555555556</v>
+        <v>0.261437908496732</v>
       </c>
       <c r="G14" t="n">
-        <v>2556</v>
+        <v>4950</v>
       </c>
       <c r="H14" t="n">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="I14" t="n">
-        <v>0.01956181533646323</v>
+        <v>0.02303030303030303</v>
       </c>
       <c r="J14" t="n">
-        <v>0.2063492063492063</v>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>**General Topic:**  Risk Management and Security Planning
-*   **Establish Comprehensive Security and Privacy Programs:** Organizations must develop, disseminate, and maintain plans for information security and privacy, including roles, responsibilities, and senior management approval.
-*   **Implement Supply Chain Risk Management:** Organizations are required to create and maintain strategies, policies, and plans to manage supply chain risks across the lifecycle of systems, components, and services, including identifying critical suppliers.
-*   **Conduct Supplier Assessments:** Organizations must assess and review supply chain-related risks associated with suppliers, including employing testing and analysis of relevant elements and processes.
-*  **Secure Supply Chain Operations:**  Organizations are required to implement operational security measures and controls to protect supply chain-related information.
-*  **Monitor and Inspect System Components:** Organizations are required to inspect systems and components to detect tampering, either randomly or at specified frequencies based on need.</t>
-        </is>
+        <v>0.4123711340206185</v>
       </c>
     </row>
     <row r="15">
@@ -3493,45 +3037,35 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['IR-7' 'PM-19' 'PM-22' 'PM-23' 'PM-24' 'PM-26' 'PM-29' 'PT-8' 'SC-21'
- 'SC-22' 'SI-18' 'SI-19']</t>
+          <t>['AC-3' 'AC-24' 'AU-10' 'CM-12' 'CM-13' 'PM-5' 'PM-20' 'PM-21' 'PM-22'
+ 'PM-26' 'PT-2' 'PT-3' 'PT-5' 'PT-6' 'PT-7' 'RA-8' 'SC-16' 'SI-14' 'SI-18'
+ 'SI-21']</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>132</v>
+        <v>380</v>
       </c>
       <c r="E15" t="n">
-        <v>26</v>
+        <v>94</v>
       </c>
       <c r="F15" t="n">
-        <v>0.196969696969697</v>
+        <v>0.2473684210526316</v>
       </c>
       <c r="G15" t="n">
-        <v>3372</v>
+        <v>5460</v>
       </c>
       <c r="H15" t="n">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="I15" t="n">
-        <v>0.009786476868327402</v>
+        <v>0.02600732600732601</v>
       </c>
       <c r="J15" t="n">
-        <v>0.4406779661016949</v>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>The general topic is **Organizational Cyber Security and Privacy Program Management**.
-Here's a summary of the regulations:
-*   **Incident Response:** Organizations must establish and automate incident response capabilities, including internal resources and coordination with external providers.
-*   **Privacy Governance:** Organizations are required to establish leadership roles for privacy, a data governance body, and a data integrity board to manage and oversee privacy-related activities.
-*   **Personally Identifiable Information (PII) Quality:** Organizations are required to implement policies and procedures for reviewing, correcting, and managing PII throughout its lifecycle, including direct collection and handling individual requests, as well as automation of these processes and data tagging.
-*   **Data De-identification:** Organizations are required to implement processes for removing or masking PII from data sets, including validating the methods used to do so and also testing to ensure data cannot be re-identified.
-*  **Risk and Complaint Management:** Organizations are required to establish risk management leadership, a risk executive function, and complaint management processes to ensure accountability and address public concerns effectively.</t>
-        </is>
+        <v>0.3983050847457627</v>
       </c>
     </row>
     <row r="16">
@@ -3543,41 +3077,30 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['AC-7' 'AC-8' 'AC-9' 'AC-11' 'AC-14' 'AC-19' 'AC-20' 'AC-22' 'MP-7'
- 'PL-4' 'SC-41']</t>
+          <t>['MA-6' 'PM-15' 'PM-25' 'SA-3' 'SA-11' 'SA-15' 'SA-22' 'SI-5' 'SI-6'
+ 'SR-4' 'SR-7']</t>
         </is>
       </c>
       <c r="D16" t="n">
         <v>110</v>
       </c>
       <c r="E16" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F16" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.2454545454545455</v>
       </c>
       <c r="G16" t="n">
         <v>3102</v>
       </c>
       <c r="H16" t="n">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="I16" t="n">
-        <v>0.02095422308188266</v>
+        <v>0.02578981302385558</v>
       </c>
       <c r="J16" t="n">
-        <v>0.3157894736842105</v>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations, grouped by topic:
-**General Topic:**  Access Control and System Usage Policies
-*   **Account &amp; Device Lockouts/Restrictions:**  These regulations focus on limiting unsuccessful login attempts through account lockouts, mobile device wipes, biometric attempt limits, and the use of alternate authentication factors. Also, implementing device locks after inactivity.
-*  **System Use Notifications:** Regulations require clear system use notifications/banners that inform users of monitoring, penalties for unauthorized use, and consent to those terms. Also, include information on successful/unsuccessful logins.
-*   **Mobile Device Controls:**  Specific requirements are mandated for mobile devices, including encryption, restrictions on connections in classified spaces, and authorization for connections to organizational systems.
-*   **External System Usage Limitations:**  These regulations impose restrictions on using external systems, controlling portable storage devices on external systems,  non-organizationally owned systems, and network accessible storage devices to protect organizational data.
-*  **User Behavior and Media Policies:**  Regulations dictate rules of behavior with social media and external website/application restrictions, policies on system media usage, and procedures for publicly accessible content to ensure information security. Additionally, controlling I/O port access.</t>
-        </is>
+        <v>0.2523364485981308</v>
       </c>
     </row>
     <row r="17">
@@ -3585,44 +3108,34 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['PL-9' 'SC-7' 'SC-18' 'SC-25' 'SC-26' 'SC-30' 'SC-35' 'SC-44' 'SI-3'
- 'SI-8' 'SI-14' 'SI-15' 'SI-21']</t>
+          <t>['AC-25' 'CP-12' 'CP-13' 'SC-3' 'SC-6' 'SC-24' 'SC-39' 'SI-13' 'SI-16'
+ 'SI-17']</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="E17" t="n">
+        <v>23</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.2555555555555555</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2830</v>
+      </c>
+      <c r="H17" t="n">
         <v>42</v>
       </c>
-      <c r="F17" t="n">
-        <v>0.2692307692307692</v>
-      </c>
-      <c r="G17" t="n">
-        <v>3640</v>
-      </c>
-      <c r="H17" t="n">
-        <v>84</v>
-      </c>
       <c r="I17" t="n">
-        <v>0.02307692307692308</v>
+        <v>0.01484098939929329</v>
       </c>
       <c r="J17" t="n">
-        <v>0.3333333333333333</v>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **System and Network Security**.
-*   **Boundary Protection:** Implement robust controls at network perimeters, including managed interfaces, traffic policies, and isolation of security functions, to prevent unauthorized access and data exfiltration.
-*   **Malicious Code &amp; Spam Protection:** Utilize mechanisms such as anti-virus, sandboxing, and spam filtering to detect, prevent, and respond to malicious code and unsolicited messages, ensuring these tools are kept up to date.
-*  **Mobile Code Control:** Define acceptable use, monitor, control the execution of mobile code, and prevent the download and automatic execution of malicious code.
-*   **System Hardening &amp; Deception:** Implement techniques such as minimal system functionality, decoys, and concealment to confuse attackers, making exploitation more difficult. Also enforce non-persistence of certain system components.
-*  **Information Management &amp; Filtering:** Employ techniques to filter information at output and refresh information at predefined frequencies, while deleting information that is no longer needed.</t>
-        </is>
+        <v>0.3538461538461539</v>
       </c>
     </row>
     <row r="18">
@@ -3630,45 +3143,34 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['AC-2' 'AC-3' 'AC-5' 'AC-6' 'AC-23' 'AC-24' 'CM-12' 'IA-2' 'IA-8' 'IA-10'
- 'IA-11' 'MA-3' 'MA-5' 'PM-5' 'SC-4' 'SC-45']</t>
+          <t>['AC-5' 'AC-8' 'AC-14' 'AU-4' 'AU-5' 'AU-6' 'AU-9' 'AU-11' 'AU-14' 'AU-16'
+ 'IA-2' 'IA-4' 'IA-5' 'IA-6' 'IA-8' 'IA-9' 'IA-10' 'IA-11' 'IA-12' 'SC-17']</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>240</v>
+        <v>380</v>
       </c>
       <c r="E18" t="n">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3041666666666666</v>
+        <v>0.2342105263157895</v>
       </c>
       <c r="G18" t="n">
-        <v>4432</v>
+        <v>5460</v>
       </c>
       <c r="H18" t="n">
-        <v>185</v>
+        <v>145</v>
       </c>
       <c r="I18" t="n">
-        <v>0.04174187725631769</v>
+        <v>0.02655677655677656</v>
       </c>
       <c r="J18" t="n">
-        <v>0.2829457364341085</v>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>The general topic of these regulations is **Access Control and Identity Management**.
-Here's a summary of the key points:
-*   **Account Lifecycle Management:** Regulations cover the full lifecycle of user accounts including creation, modification, enabling, disabling, and removal, with a focus on automated processes, temporary accounts, inactivity, and privileged accounts.
-*   **Access Enforcement:** Enforce access control policies, including mandatory, discretionary, role-based, and attribute-based access control, as well as dual authorization, control over information release, and audited overrides of controls.
-*   **Least Privilege and Separation of Duties:** The regulations emphasize the principles of least privilege, separation of duties, and limiting privileged access to specific personnel and functions, preventing unauthorized execution of privileged functions.
-*   **Identification and Authentication:** Regulations mandate unique identification and authentication of organizational and non-organizational users, with multi-factor authentication for both privileged and non-privileged accounts, single sign-on capabilities, and requirements for accepting PIV credentials.
-*   **System and Maintenance Controls:** These include controlled use of system maintenance tools, inspection of tools and media for malicious code, personnel authorization for maintenance, and inventory control for both systems and personal information to protect against data breaches.</t>
-        </is>
+        <v>0.3803418803418803</v>
       </c>
     </row>
     <row r="19">
@@ -3676,45 +3178,33 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['AC-25' 'PL-7' 'PL-8' 'PM-25' 'SA-2' 'SA-3' 'SA-4' 'SA-5' 'SA-8' 'SA-9'
- 'SA-11' 'SA-15' 'SA-17' 'SC-2' 'SC-3' 'SC-32' 'SC-39' 'SI-16' 'SR-3'
- 'SR-5' 'SR-9']</t>
+          <t>['AC-20' 'MA-3' 'MP-6' 'MP-7' 'SC-41' 'SI-19' 'SR-12']</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>420</v>
+        <v>42</v>
       </c>
       <c r="E19" t="n">
-        <v>140</v>
+        <v>12</v>
       </c>
       <c r="F19" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2857142857142857</v>
       </c>
       <c r="G19" t="n">
-        <v>5712</v>
+        <v>2002</v>
       </c>
       <c r="H19" t="n">
-        <v>198</v>
+        <v>40</v>
       </c>
       <c r="I19" t="n">
-        <v>0.03466386554621849</v>
+        <v>0.01998001998001998</v>
       </c>
       <c r="J19" t="n">
-        <v>0.4142011834319527</v>
-      </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>**General Topic:** Secure System Development and Acquisition
-*   **Holistic Security and Privacy Integration:** Regulations emphasize incorporating security and privacy considerations throughout the entire system development lifecycle (SDLC), from initial concept through acquisition and maintenance. This includes establishing clear roles, responsibilities, and documentation.
-*   **Defense-in-Depth Architecture:** Requirements focus on designing systems with layered security using multiple controls allocated across different architectural locations and layers and by using multiple vendors. This includes concepts such as process isolation, memory protection, and separating system and user functionality.
-*   **Rigorous Development Practices:** Regulations mandate secure coding practices, testing protocols (including static, dynamic, and penetration testing), and continuous improvement processes. This also includes supply chain risk management, with requirements around diverse supply bases, sub-tier flow-down, and tamper protection.
-*  **Specific Security Engineering Principles:** Numerous regulations detail specific security engineering principles that must be applied, such as least privilege, minimized sharing, secure defaults, and continuous protection.
-*   **Acquisition Controls:** The regulations extensively cover the acquisition process, mandating requirements for security and privacy functional criteria in contracts, descriptions of control properties, documentation, and the use of approved information assurance products and services. It also emphasizes the need to control external service providers and verify their compliance with organizational requirements.</t>
-        </is>
+        <v>0.2307692307692308</v>
       </c>
     </row>
     <row r="20">
@@ -3722,45 +3212,34 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['AC-18' 'CA-9' 'IR-4' 'IR-6' 'PE-17' 'PM-16' 'SC-27' 'SC-29' 'SC-43'
- 'SR-8']</t>
+          <t>['CA-3' 'PL-2' 'PL-7' 'PL-8' 'PL-10' 'PL-11' 'PM-1' 'PM-7' 'PM-11' 'PM-17'
+ 'PM-32' 'RA-2' 'RA-3' 'RA-9' 'SA-2' 'SA-9' 'SR-2']</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>90</v>
+        <v>272</v>
       </c>
       <c r="E20" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="F20" t="n">
-        <v>0.1666666666666667</v>
+        <v>0.2757352941176471</v>
       </c>
       <c r="G20" t="n">
-        <v>2830</v>
+        <v>4692</v>
       </c>
       <c r="H20" t="n">
-        <v>71</v>
+        <v>134</v>
       </c>
       <c r="I20" t="n">
-        <v>0.02508833922261484</v>
+        <v>0.02855924978687127</v>
       </c>
       <c r="J20" t="n">
-        <v>0.1744186046511628</v>
-      </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>The general topic for all of these regulations is **Cybersecurity and Incident Response Management**.
-Here's a summary of the key points:
-*   **Secure Wireless and Internal Connections:** Regulations mandate secure configurations, authentication, encryption, limited access, and disabling unused wireless capabilities. Similarly, internal system connections require authorization, documentation, termination conditions, and regular reviews.
-*   **Comprehensive Incident Handling:** Organizations must implement a robust incident handling capability covering preparation, detection, containment, eradication, and recovery, with continuous improvement, automated processes, and dynamic reconfiguration options.
-*   **Incident Coordination &amp; Reporting:** Requires coordination with both internal and external entities, including supply chains, for incident handling, information sharing, and reporting. Includes requirements for an integrated response team and incident analysis (forensic, behavior). Also covers public relations.
-*   **Threat Awareness &amp; Preparedness:** Emphasizes proactive measures like threat awareness programs, use of automated mechanisms for threat intelligence, alternate work sites with security controls, and platform heterogeneity to enhance resilience.
-*  **Usage Control &amp; Notifications:** Requires restrictions on the use of certain system components, and the establishment of notification procedures for supply chain compromises, assessments, and other critical information.</t>
-        </is>
+        <v>0.3588516746411483</v>
       </c>
     </row>
     <row r="21">
@@ -3772,40 +3251,30 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['CM-13' 'PL-2' 'PL-10' 'PL-11' 'PM-7' 'PM-10' 'PM-11' 'PM-27' 'PM-32'
- 'RA-2' 'RA-8' 'RA-9' 'SA-20' 'SA-22' 'SA-23']</t>
+          <t>['SC-5' 'SC-7' 'SC-18' 'SC-20' 'SC-21' 'SC-22' 'SC-26' 'SC-35' 'SC-43'
+ 'SC-44' 'SC-48' 'SI-3' 'SI-4' 'SI-8' 'SI-15']</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>210</v>
       </c>
       <c r="E21" t="n">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F21" t="n">
-        <v>0.2</v>
+        <v>0.280952380952381</v>
       </c>
       <c r="G21" t="n">
         <v>4170</v>
       </c>
       <c r="H21" t="n">
-        <v>81</v>
+        <v>131</v>
       </c>
       <c r="I21" t="n">
-        <v>0.01942446043165467</v>
+        <v>0.03141486810551559</v>
       </c>
       <c r="J21" t="n">
-        <v>0.3414634146341464</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>**General Topic:** System Security and Privacy Management
-*   **Establish Comprehensive Documentation:** Develop and maintain thorough documentation, including data action maps, system security and privacy plans, and enterprise architecture, all of which consider information security and privacy impacts.
-*   **Implement Risk-Based Approach:**  Incorporate risk management processes into authorization, mission, and business process definitions, using security categorization and impact-level prioritization to tailor controls appropriately.
-*   **Conduct Privacy Assessments and Reporting:** Conduct privacy impact assessments before processing personally identifiable information, and develop regular privacy reports to ensure accountability and demonstrate compliance.
-*   **Manage System Components:** Analyze, prioritize, customize and ensure support of critical system components, and replace or find alternative support for components that are no longer supported by vendors.
-*   **Ensure System Integrity:**  Verify that systems are used for their intended purpose and employ specialization techniques to increase the trustworthiness of mission-essential systems or components.</t>
-        </is>
+        <v>0.3105263157894737</v>
       </c>
     </row>
   </sheetData>
@@ -3819,7 +3288,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -3833,6 +3302,771 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Divisive_Communities</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>number of regulations</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>names of regulations</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>possible inside relations</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>actual inside relations</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>percentage inside relations</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>possible outside relations</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>actual outside relations</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>percentage outside relations</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>inner connections probability</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CM-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1'
+ 'PE-1' 'PL-1' 'PM-2' 'PM-6' 'PM-9' 'PM-29' 'PS-1' 'PS-8' 'RA-1' 'SA-1'
+ 'SC-1' 'SI-1' 'SI-12' 'SR-1']</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>552</v>
+      </c>
+      <c r="E2" t="n">
+        <v>79</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.1431159420289855</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6456</v>
+      </c>
+      <c r="H2" t="n">
+        <v>63</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.009758364312267658</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.5563380281690141</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>227</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['AC-2' 'AC-3' 'AC-4' 'AC-5' 'AC-6' 'AC-7' 'AC-8' 'AC-9' 'AC-11' 'AC-14'
+ 'AC-16' 'AC-17' 'AC-18' 'AC-19' 'AC-20' 'AC-21' 'AC-22' 'AC-23' 'AC-24'
+ 'AC-25' 'AT-2' 'AT-3' 'AT-4' 'AU-2' 'AU-3' 'AU-4' 'AU-5' 'AU-6' 'AU-7'
+ 'AU-8' 'AU-9' 'AU-10' 'AU-11' 'AU-12' 'AU-13' 'AU-14' 'AU-16' 'CA-2'
+ 'CA-3' 'CA-5' 'CA-6' 'CA-7' 'CA-8' 'CA-9' 'CM-2' 'CM-3' 'CM-4' 'CM-5'
+ 'CM-6' 'CM-7' 'CM-8' 'CM-9' 'CM-10' 'CM-11' 'CM-12' 'CM-13' 'CM-14'
+ 'CP-2' 'CP-3' 'CP-4' 'CP-6' 'CP-7' 'CP-8' 'CP-9' 'CP-10' 'IA-2' 'IA-3'
+ 'IA-4' 'IA-5' 'IA-6' 'IA-7' 'IA-8' 'IA-9' 'IA-10' 'IA-11' 'IA-12' 'IR-2'
+ 'IR-3' 'IR-4' 'IR-5' 'IR-6' 'IR-7' 'IR-8' 'IR-9' 'MA-2' 'MA-3' 'MA-4'
+ 'MA-5' 'MA-6' 'MA-7' 'MP-2' 'MP-3' 'MP-4' 'MP-5' 'MP-6' 'MP-7' 'PE-2'
+ 'PE-3' 'PE-4' 'PE-5' 'PE-6' 'PE-8' 'PE-11' 'PE-12' 'PE-13' 'PE-14'
+ 'PE-16' 'PE-17' 'PE-22' 'PL-2' 'PL-4' 'PL-8' 'PL-9' 'PL-10' 'PL-11'
+ 'PM-1' 'PM-4' 'PM-5' 'PM-7' 'PM-8' 'PM-10' 'PM-11' 'PM-12' 'PM-13'
+ 'PM-14' 'PM-16' 'PM-17' 'PM-18' 'PM-20' 'PM-21' 'PM-22' 'PM-23' 'PM-25'
+ 'PM-26' 'PM-28' 'PM-30' 'PM-31' 'PM-32' 'PS-2' 'PS-3' 'PS-4' 'PS-5'
+ 'PS-6' 'PS-7' 'PT-1' 'PT-2' 'PT-3' 'PT-4' 'PT-5' 'PT-6' 'PT-7' 'RA-2'
+ 'RA-3' 'RA-5' 'RA-7' 'RA-8' 'RA-9' 'SA-3' 'SA-4' 'SA-5' 'SA-8' 'SA-9'
+ 'SA-10' 'SA-11' 'SA-15' 'SA-16' 'SA-17' 'SA-20' 'SA-21' 'SA-22' 'SA-23'
+ 'SC-2' 'SC-3' 'SC-4' 'SC-5' 'SC-7' 'SC-8' 'SC-11' 'SC-12' 'SC-13' 'SC-15'
+ 'SC-16' 'SC-17' 'SC-18' 'SC-23' 'SC-26' 'SC-28' 'SC-31' 'SC-32' 'SC-34'
+ 'SC-35' 'SC-36' 'SC-37' 'SC-38' 'SC-39' 'SC-42' 'SC-43' 'SC-44' 'SC-45'
+ 'SC-46' 'SC-47' 'SC-48' 'SC-49' 'SC-50' 'SI-2' 'SI-3' 'SI-4' 'SI-6'
+ 'SI-7' 'SI-8' 'SI-10' 'SI-11' 'SI-13' 'SI-15' 'SI-16' 'SI-18' 'SI-19'
+ 'SR-2' 'SR-3' 'SR-4' 'SR-5' 'SR-6' 'SR-7' 'SR-8' 'SR-9' 'SR-10' 'SR-11']</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>51302</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2746</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.05352617831663483</v>
+      </c>
+      <c r="G3" t="n">
+        <v>14982</v>
+      </c>
+      <c r="H3" t="n">
+        <v>149</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.009945267654518756</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.94853195164076</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['AC-10']</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>292</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.003424657534246575</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['AC-12' 'SC-10' 'SI-14' 'SI-21']</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1156</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.005190311418685121</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['CP-11' 'CP-13']</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>582</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.006872852233676976</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['CP-12' 'SC-20' 'SC-21' 'SC-22' 'SC-24' 'SI-17']</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>30</v>
+      </c>
+      <c r="E7" t="n">
+        <v>13</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.4333333333333333</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1722</v>
+      </c>
+      <c r="H7" t="n">
+        <v>16</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.009291521486643438</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.4482758620689655</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['PE-9']</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>292</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.003424657534246575</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['PE-10' 'PE-15']</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>582</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.001718213058419244</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['PE-18' 'PE-19' 'PE-20' 'PE-21' 'PE-23' 'SC-40']</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>30</v>
+      </c>
+      <c r="E10" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1722</v>
+      </c>
+      <c r="H10" t="n">
+        <v>16</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.009291521486643438</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['PL-7' 'PM-3' 'SA-2']</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="G11" t="n">
+        <v>870</v>
+      </c>
+      <c r="H11" t="n">
+        <v>7</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.008045977011494253</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.3636363636363636</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['PM-15' 'SI-5']</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>582</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.005154639175257732</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>4</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['PM-19' 'PM-24' 'PM-27' 'PT-8']</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1156</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.006055363321799308</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.4615384615384616</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['PS-9']</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>292</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['RA-6' 'RA-10']</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G15" t="n">
+        <v>582</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.01030927835051546</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>['SC-6']</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
+        <v>292</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.003424657534246575</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['SC-25' 'SC-30']</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>582</v>
+      </c>
+      <c r="H17" t="n">
+        <v>6</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.01030927835051546</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['SC-27' 'SC-29']</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>582</v>
+      </c>
+      <c r="H18" t="n">
+        <v>4</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.006872852233676976</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['SC-41']</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
+        <v>292</v>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.00684931506849315</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['SI-20']</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="n">
+        <v>292</v>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.003424657534246575</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['SR-12']</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>292</v>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" t="n">
+        <v>0.003424657534246575</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
           <t>Label_propagation</t>
         </is>
       </c>
@@ -3879,11 +4113,6 @@
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>inner connections probability</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
         </is>
       </c>
     </row>
@@ -3950,18 +4179,6 @@
       <c r="J2" t="n">
         <v>0.9996839443742098</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations, categorized by their general topic, in concise bullet points:
-**General Topic: Cyber Security and Privacy Controls**
-*   **Policy and Procedure Foundation:** Establish and maintain documented policies and procedures for various aspects of cyber security and privacy, including access control, awareness and training, audit, incident response, configuration, maintenance, media protection, physical security, planning, personnel security, supply chain, and personally identifiable information (PII) processing.
-*   **Access Control &amp; Identity Management:** Manage user accounts, enforce least privilege, implement multi-factor authentication, control access based on roles and attributes, and secure remote and wireless access. Additionally establish unique device identities, restrict access for high-risk individuals and implement controls that prevent information flow between different security domains.
-*   **System Integrity and Protection:** Implement controls for software and firmware updates, malicious code protection, denial-of-service prevention, resource availability, and system monitoring. Protect data during transmission and at rest. 
-*   **Security and Privacy Awareness and Training:** Provide regular security and privacy training for all users, including role-based training for specific responsibilities, and awareness training for insider threats and social engineering.
-*  **Auditing and Incident Response:** Implement comprehensive logging, monitor for system breaches and unauthorized access, and develop incident response plans, that include a robust incident handling capacity, and test plans regularly.
-These points encapsulate the core elements of the cyber regulations provided, which cover a very broad range of controls.</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -3995,14 +4212,6 @@
       </c>
       <c r="J3" t="n">
         <v>0.6666666666666666</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>**Topic:** Physical Security and Environmental Controls
-*   **Emergency Power Shutoff:** Systems must have the capability to shut off power in emergencies, with accessible and protected shutoff devices.
-*   **Water Leakage Protection:** Systems must be protected from water damage via accessible shutoff valves known to key personnel.
-*   **Automated Water Detection:** Systems should include automated mechanisms to detect water near the system and alert designated personnel.</t>
-        </is>
       </c>
     </row>
   </sheetData>
@@ -4010,13 +4219,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -4076,11 +4285,6 @@
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>inner connections probability</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Summary</t>
         </is>
       </c>
     </row>
@@ -4145,17 +4349,6 @@
       <c r="J2" t="n">
         <v>0.9910485933503836</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulations, organized by topic:
-**General Topic: Comprehensive Cybersecurity and Privacy Controls**
-*   **Access Control &amp; Account Management:** These regulations focus on controlling user access, managing accounts (creation, modification, disabling, and monitoring), implementing least privilege, and enforcing policies for both privileged and non-privileged accounts. They also address dynamic privilege management and restrictions on shared accounts.
-*   **Information Flow Control:** The regulations detail how to manage the flow of information within and between systems. This includes enforcing policies based on attributes, metadata, and domain separation, along with strict rules for encrypted data, one-way flows, and sanitization.
-*   **System &amp; Information Integrity:** These regulations emphasize protecting data and system integrity through flaw remediation, malicious code protection, system monitoring, software and firmware integrity checks, input validation, error handling, and memory protection.  They also cover requirements to detect and manage vulnerabilities.
-*   **Security &amp; Privacy Planning:** These controls require documented security, privacy, and supply chain risk management plans. They include the need for risk assessments, security categorizations, continuous monitoring, incident response and contingency planning, and employee training. The regulations ensure both security and privacy are included in all aspects of the system, especially as it relates to PII.
-*  **Physical Security &amp; Personnel:** These controls focus on physical access authorization and control, monitoring and visitor access. It also addresses requirements around emergency power and environmental control. They also require personnel security measures including screening, termination procedures, and access agreements to ensure personnel are trustworthy and meet security needs.</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -4188,15 +4381,6 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**Topic: Access Control**
-*   **Limits Concurrent Sessions:** This regulation mandates limiting the number of simultaneous logins for specific user accounts or account types.
-*   **Organization-Defined Limits:** The specific limits on concurrent sessions are determined by the organization.
-*   **Enforces Single User Principle:** Aims to reduce the risk of multiple users sharing credentials and helps identify anomalous activity more easily.</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -4229,15 +4413,6 @@
       <c r="J4" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>**Topic:** Session Management
-*   **Automatic Session Termination:** Mandates automatic termination of user sessions based on predefined conditions or trigger events.
-*   **User-Initiated Logout:** Requires a logout function for users to manually end authenticated sessions.
-*   **Logout Confirmation:** Demands a clear message confirming session termination to users upon logout.
-*   **Timeout Warning:** Requires a message to be displayed, warning users of imminent session expiration due to timeout.</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -4272,16 +4447,6 @@
       <c r="J5" t="n">
         <v>0.3333333333333333</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>**Topic:** Business Continuity and Resilience
-*   **Alternative Communication:** Organizations must have backup communication protocols to maintain operations during disruptions.
-*   **Backup Security:** Organizations must have alternative security measures ready if primary security controls fail.
-*   **Flexibility:** Regulations emphasize the need for flexibility in both communication and security.
-*   **Defined Alternatives:** Organizations are responsible for defining what their specific alternative communication and security measures are.
-*   **Contingency Planning:** These regulations are part of a broader business continuity and contingency planning strategy.</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -4314,14 +4479,6 @@
       <c r="J6" t="n">
         <v>0</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>**Topic:** Power System Security
-*   Protect power equipment and cabling from damage.
-*   Utilize redundant power cabling paths separated by a defined distance.
-*   Implement automatic voltage controls for critical system components.</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -4356,14 +4513,6 @@
       <c r="J7" t="n">
         <v>0.6666666666666666</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>**General Topic:** Physical Security and Environmental Controls
-*   **Emergency Power Shutoff:** Systems must have emergency shutoff capabilities, with accessible switches located appropriately and protected from unauthorized use.
-*   **Water Damage Prevention:** Implement master shutoff valves to protect systems from water damage, ensuring they are accessible, functional, and known to key personnel.
-*  **Water Detection and Alerting:** Use automated mechanisms to detect water near systems and promptly alert designated personnel.</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -4398,14 +4547,6 @@
       <c r="J8" t="n">
         <v>0.5</v>
       </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>**Topic:** Cyber Governance and Leadership Roles
-*   **Senior Information Security Officer:** Requires a designated senior leader responsible for the organization-wide information security program.
-*   **Senior Accountable Official for Risk Management:** Mandates a senior leader to align security and privacy with strategic and financial planning.
-*   **Risk Executive Function:** Establishes a function to oversee and ensure consistent risk management across the organization.</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -4440,16 +4581,6 @@
       <c r="J9" t="n">
         <v>0.4</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>**General Topic:** Security Information and Communication
-*   Establish contact with security and privacy groups for ongoing education, best practices, and information sharing.
-*   Receive and generate security alerts, advisories, and directives from external and internal sources.
-*   Disseminate security alerts, advisories, and directives to defined personnel, internal elements, or external organizations.
-*   Implement security directives within established timeframes or notify noncompliance.
-*   Utilize automated mechanisms to broadcast security alerts and advisory information throughout the organization.</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -4482,13 +4613,6 @@
       <c r="J10" t="n">
         <v>0</v>
       </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**Topic:** Organizational Security Roles and Responsibilities
-*   **Security and Privacy Integration:** Mandates the inclusion of security and privacy responsibilities within all relevant position descriptions.</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -4521,16 +4645,6 @@
       <c r="J11" t="n">
         <v>0</v>
       </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>**Topic: Computer Matching Program Requirements**
-*   Requires Data Integrity Board approval before initiating a matching program.
-*   Mandates a formal computer matching agreement between participating entities.
-*   Requires public notification of the matching program through the Federal Register.
-*   Stipulates independent verification of matching results before adverse actions are taken.
-*   Guarantees individuals notice and the opportunity to contest findings before adverse action.</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -4563,15 +4677,6 @@
       <c r="J12" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**General Topic:** Technical Surveillance Countermeasures
-*   **Regular Surveys:** Organizations must conduct technical surveillance countermeasures surveys at specific locations.
-*  **Frequency Defined:** The frequency of these surveys is determined by the organization.
-*  **Triggered Surveys:** Surveys must also be conducted when certain events or indicators occur, as defined by the organization.</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -4604,17 +4709,6 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of that regulation:
-**Topic:** System and Component Security
-*   **Specialized Security Measures:** Focuses on implementing specific security measures on critical systems or components.
-*   **Tailored Modifications:** Requires design, modification, or augmentation of systems to enhance security.
-*   **Mission-Critical Focus:** Specifically targets systems supporting essential services or functions.
-*   **Trustworthiness Goal:** Aims to increase the reliability and security of those systems.
-*   **Organization-Defined Scope:** The specific systems or components to be protected are determined by the organization.</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -4647,17 +4741,6 @@
       <c r="J14" t="n">
         <v>0</v>
       </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**Topic:** Resource Management
-*   **Focus on Availability:** The regulation emphasizes maintaining the availability of resources.
-*   **Resource Allocation:** It mandates the allocation of resources as defined by the organization.
-*   **Control Mechanisms:** Requires the use of controls such as priority or quota based systems to maintain availability.
-*   **Organization-Defined:** The organization has the responsibility to define what resources are controlled and the exact control mechanisms.
-*   **Flexible Implementation:** The regulation allows for flexibility in how organizations choose to implement controls.</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -4690,16 +4773,6 @@
       <c r="J15" t="n">
         <v>0</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**Topic:** System Security Hardening
-*   **Minimize Functionality:** Limit the features and services running on specified system components.
-*   **Reduce Data Storage:** Restrict the amount of information stored on the targeted components.
-*   **Focus:** Applies to organization-defined system components.
-*   **Goal:** Enhance security posture by reducing attack surface and potential impact from breaches.</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -4732,14 +4805,6 @@
       <c r="J16" t="n">
         <v>0</v>
       </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**General Topic:** System Security Configuration
-*   **Platform-Independent Applications:** Organizations must include specified platform-independent applications within their systems.
-*   **Organization-Defined List:** The specific applications are determined by the organization itself.</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -4772,17 +4837,6 @@
       <c r="J17" t="n">
         <v>0</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**General Topic: System Access Control**
-*   **Physical/Logical Disablement:** Requires the disabling or removal of specific connection ports or I/O devices.
-*   **Scope:** Applies to organization-defined systems or components.
-*   **Control Type:** Focuses on both physical and logical access points.
-*   **Objective:** Limits potential attack vectors through I/O.
-*   **Customization:** Implementation is tailored to the specific organization's needs and infrastructure.</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -4815,17 +4869,6 @@
       <c r="J18" t="n">
         <v>0</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**Topic:** Communication Security and Resilience
-*   **Alternate Communication:** Requires the establishment of backup communication methods.
-*   **Operational Continuity:** Ensures continued system operations during primary communication disruptions.
-*   **Command and Control:** Supports organizational command and control functions.
-*   **Resilience:** Increases the organization's ability to operate even when main communication methods are unavailable.
-*   **Defined Paths**:  Specific paths must be established, not just a general idea of alternatives.</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -4860,16 +4903,6 @@
       <c r="J19" t="n">
         <v>0.4</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>**Topic:** System and Information Non-Persistence
-*   System components and services should be non-persistent, starting in a known state and terminating after use or periodically.
-*   Software and data for system refreshes must come from defined trusted sources.
-*   Information should be refreshed or generated on demand and deleted when no longer needed.
-*   System connections should be established on demand and terminated after use or inactivity.
-*   Information should be refreshed at defined frequencies or generated on demand, and then deleted when no longer needed.</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -4902,14 +4935,6 @@
       <c r="J20" t="n">
         <v>0</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided regulation:
-**General Topic:** Data Loss Prevention and Detection
-*   **Data Tainting:** Organizations must embed data or capabilities into specified systems to track potential data exfiltration or improper removal.
-*   **Customizable Application:** The systems and components where "tainting" is applied are defined by the organization.</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -4941,17 +4966,6 @@
       </c>
       <c r="J21" t="n">
         <v>0</v>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>Okay, here's a summary of the provided cyber regulation:
-**Topic:** Secure Data and Component Disposal
-*   **Mandates Secure Disposal:** Requires organizations to dispose of sensitive data, documentation, tools, and system components securely.
-*   **Organization-Defined Methods:** The specific disposal techniques and methods are to be defined by the organization itself.
-*   **Flexibility in Implementation:** Allows for organizational flexibility in choosing appropriate disposal methods, likely based on risk and sensitivity.
-*   **Focus on Protecting Sensitive Assets:** The goal is to prevent unauthorized access to sensitive information during disposal.
-*   **Applies to Various Assets:** Includes data, documentation, tools, and system components in the disposal requirement.</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a parameter for minimal number of  different relations per sub-regulation
</commit_message>
<xml_diff>
--- a/regulations outputs/in family connection statistics test old.xlsx
+++ b/regulations outputs/in family connection statistics test old.xlsx
@@ -549,10 +549,10 @@
         <v>51</v>
       </c>
       <c r="D4" t="n">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" t="n">
         <v>2</v>
@@ -577,10 +577,10 @@
         <v>33.33880907405347</v>
       </c>
       <c r="D5" t="n">
-        <v>16.43602315473111</v>
+        <v>17.04336206492694</v>
       </c>
       <c r="E5" t="n">
-        <v>3.963982580024393</v>
+        <v>3.660241579602723</v>
       </c>
       <c r="F5" t="n">
         <v>50.23971484163124</v>
@@ -605,10 +605,10 @@
         <v>63</v>
       </c>
       <c r="D6" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E6" t="n">
-        <v>4.25</v>
+        <v>5.25</v>
       </c>
       <c r="F6" t="n">
         <v>3</v>
@@ -661,10 +661,10 @@
         <v>1.255508040619211</v>
       </c>
       <c r="D8" t="n">
-        <v>2.546670959458601</v>
+        <v>2.455920533618159</v>
       </c>
       <c r="E8" t="n">
-        <v>3.695778097972835</v>
+        <v>4.002468056108496</v>
       </c>
       <c r="F8" t="n">
         <v>0.2916019735816703</v>
@@ -689,10 +689,10 @@
         <v>0.8095238095238095</v>
       </c>
       <c r="D9" t="n">
-        <v>2.235294117647059</v>
+        <v>1.44</v>
       </c>
       <c r="E9" t="n">
-        <v>3.294117647058823</v>
+        <v>2.857142857142857</v>
       </c>
       <c r="F9" t="n">
         <v>0.6666666666666666</v>
@@ -717,10 +717,10 @@
         <v>1812</v>
       </c>
       <c r="D10" t="n">
-        <v>1699</v>
+        <v>1679</v>
       </c>
       <c r="E10" t="n">
-        <v>1089</v>
+        <v>1123</v>
       </c>
       <c r="F10" t="n">
         <v>2872</v>
@@ -745,10 +745,10 @@
         <v>1355</v>
       </c>
       <c r="D11" t="n">
-        <v>1468</v>
+        <v>1488</v>
       </c>
       <c r="E11" t="n">
-        <v>2078</v>
+        <v>2044</v>
       </c>
       <c r="F11" t="n">
         <v>295</v>
@@ -773,10 +773,10 @@
         <v>0.5721502999684244</v>
       </c>
       <c r="D12" t="n">
-        <v>0.5364698452794443</v>
+        <v>0.530154720555731</v>
       </c>
       <c r="E12" t="n">
-        <v>0.3438585412061888</v>
+        <v>0.3545942532365014</v>
       </c>
       <c r="F12" t="n">
         <v>0.9068519103252289</v>
@@ -801,10 +801,10 @@
         <v>0.5018879211466615</v>
       </c>
       <c r="D13" t="n">
-        <v>0.5067462243624968</v>
+        <v>0.5054518804352141</v>
       </c>
       <c r="E13" t="n">
-        <v>0.3343530149871812</v>
+        <v>0.3459383241993728</v>
       </c>
       <c r="F13" t="n">
         <v>0.283225557162202</v>
@@ -829,10 +829,10 @@
         <v>0.09721030042918455</v>
       </c>
       <c r="D14" t="n">
-        <v>0.125</v>
+        <v>0.1224296339507073</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2533736621684504</v>
+        <v>0.2639868359191349</v>
       </c>
       <c r="F14" t="n">
         <v>0.05527754253599199</v>
@@ -857,10 +857,10 @@
         <v>0.1882305960895143</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1268314687412245</v>
+        <v>0.1296417990023628</v>
       </c>
       <c r="E15" t="n">
-        <v>0.2608524825707488</v>
+        <v>0.2648086755865393</v>
       </c>
       <c r="F15" t="n">
         <v>0.6099981118214579</v>
@@ -885,10 +885,10 @@
         <v>0.02024926773865742</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02039908843310544</v>
+        <v>0.02071211825951393</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02557286667158926</v>
+        <v>0.02514083294383902</v>
       </c>
       <c r="F16" t="n">
         <v>0.008779761904761905</v>
@@ -913,10 +913,10 @@
         <v>0.01635676483684854</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01961080884063076</v>
+        <v>0.01981114222931618</v>
       </c>
       <c r="E17" t="n">
-        <v>0.02549699696328481</v>
+        <v>0.02505115812943544</v>
       </c>
       <c r="F17" t="n">
         <v>0.006139402141691993</v>
@@ -941,10 +941,10 @@
         <v>0.6552129715014351</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7194055526353513</v>
+        <v>0.7106068922630533</v>
       </c>
       <c r="E18" t="n">
-        <v>0.8166468191740512</v>
+        <v>0.826091822739013</v>
       </c>
       <c r="F18" t="n">
         <v>0.7258778844532167</v>
@@ -969,10 +969,10 @@
         <v>0.8400999478874375</v>
       </c>
       <c r="D19" t="n">
-        <v>0.7321701196613918</v>
+        <v>0.7348845453820096</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8219169316823961</v>
+        <v>0.8271498481988205</v>
       </c>
       <c r="F19" t="n">
         <v>0.9800713249800299</v>
@@ -997,10 +997,10 @@
         <v>0.7610834937156346</v>
       </c>
       <c r="D20" t="n">
-        <v>0.732909810276525</v>
+        <v>0.7291942485825862</v>
       </c>
       <c r="E20" t="n">
-        <v>0.8225427253300422</v>
+        <v>0.8257922735461877</v>
       </c>
       <c r="F20" t="n">
         <v>0.9443570584316672</v>
@@ -2243,40 +2243,37 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['AC-2' 'AC-3' 'AC-4' 'AC-5' 'AC-6' 'AC-7' 'AC-8' 'AC-9' 'AC-11' 'AC-14'
- 'AC-17' 'AC-18' 'AC-20' 'AC-22' 'AC-23' 'AU-2' 'AU-3' 'AU-4' 'AU-5'
- 'AU-6' 'AU-7' 'AU-8' 'AU-11' 'AU-12' 'AU-13' 'AU-14' 'AU-16' 'CA-9'
- 'CM-3' 'CM-5' 'CM-11' 'IA-2' 'IA-3' 'IA-4' 'IA-5' 'IA-6' 'IA-8' 'IA-9'
- 'IA-10' 'IA-11' 'IA-12' 'MA-4' 'MA-5' 'MA-7' 'PE-2' 'PE-3' 'PE-5' 'PE-8'
- 'PE-17' 'PE-22' 'PL-4' 'PM-12' 'PS-2' 'PS-3' 'PS-4' 'PS-5' 'PS-6' 'PS-7'
- 'PT-8' 'SA-21' 'SC-15' 'SC-31' 'SC-37' 'SC-45' 'SC-46' 'SC-48' 'SI-4'
- 'SI-10' 'SI-11' 'SI-15' 'SI-20']</t>
+          <t>['AC-3' 'AC-16' 'AC-21' 'AT-2' 'AT-3' 'AT-4' 'CM-13' 'CP-3' 'CP-4' 'IR-2'
+ 'IR-3' 'IR-4' 'IR-6' 'IR-7' 'IR-8' 'IR-9' 'MP-6' 'PE-10' 'PE-15' 'PE-22'
+ 'PM-2' 'PM-5' 'PM-13' 'PM-14' 'PM-19' 'PM-20' 'PM-21' 'PM-22' 'PM-23'
+ 'PM-24' 'PM-26' 'PM-27' 'PM-29' 'PS-9' 'PT-1' 'PT-2' 'PT-3' 'PT-4' 'PT-5'
+ 'PT-6' 'PT-7' 'PT-8' 'RA-8' 'SA-16' 'SC-42' 'SI-18' 'SI-19' 'SR-12']</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4970</v>
+        <v>2256</v>
       </c>
       <c r="E2" t="n">
-        <v>588</v>
+        <v>259</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1183098591549296</v>
+        <v>0.1148049645390071</v>
       </c>
       <c r="G2" t="n">
-        <v>15762</v>
+        <v>11760</v>
       </c>
       <c r="H2" t="n">
-        <v>350</v>
+        <v>210</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02220530389544474</v>
+        <v>0.01785714285714286</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6268656716417911</v>
+        <v>0.5522388059701493</v>
       </c>
     </row>
     <row r="3">
@@ -2284,35 +2281,36 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CM-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1'
- 'PE-1' 'PL-1' 'PL-7' 'PM-2' 'PM-9' 'PM-29' 'PS-1' 'PS-8' 'PT-1' 'RA-1'
- 'SA-1' 'SC-1' 'SC-42' 'SI-1' 'SI-12' 'SR-1']</t>
+          <t>['AC-10' 'AC-12' 'AC-24' 'AC-25' 'AU-9' 'AU-10' 'CM-2' 'CM-3' 'CM-5'
+ 'CM-9' 'CM-11' 'CM-14' 'CP-9' 'IA-7' 'MP-2' 'MP-3' 'MP-4' 'MP-5' 'PE-4'
+ 'PE-9' 'SC-8' 'SC-10' 'SC-11' 'SC-12' 'SC-13' 'SC-16' 'SC-17' 'SC-20'
+ 'SC-23' 'SC-28' 'SC-34' 'SI-10' 'SI-14' 'SI-16' 'SI-21']</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>650</v>
+        <v>1190</v>
       </c>
       <c r="E3" t="n">
-        <v>83</v>
+        <v>158</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1276923076923077</v>
+        <v>0.1327731092436975</v>
       </c>
       <c r="G3" t="n">
-        <v>6942</v>
+        <v>9030</v>
       </c>
       <c r="H3" t="n">
-        <v>67</v>
+        <v>212</v>
       </c>
       <c r="I3" t="n">
-        <v>0.00965139729184673</v>
+        <v>0.02347729789590255</v>
       </c>
       <c r="J3" t="n">
-        <v>0.5533333333333333</v>
+        <v>0.4270270270270271</v>
       </c>
     </row>
     <row r="4">
@@ -2320,36 +2318,35 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['AC-10' 'AC-12' 'AC-16' 'AC-19' 'AC-24' 'AU-9' 'AU-10' 'CM-14' 'CP-6'
- 'CP-9' 'CP-10' 'IA-7' 'MP-2' 'MP-3' 'MP-4' 'MP-5' 'MP-7' 'PE-4' 'PE-9'
- 'SC-8' 'SC-10' 'SC-11' 'SC-12' 'SC-13' 'SC-16' 'SC-17' 'SC-20' 'SC-23'
- 'SC-28' 'SC-34' 'SC-36' 'SC-41' 'SI-3' 'SI-14' 'SI-21']</t>
+          <t>['CP-2' 'CP-6' 'CP-7' 'CP-8' 'CP-10' 'CP-11' 'CP-12' 'CP-13' 'PE-11'
+ 'PE-12' 'PE-13' 'PE-18' 'PE-19' 'PE-20' 'PE-21' 'PE-23' 'PM-8' 'SC-6'
+ 'SC-24' 'SC-36' 'SC-47' 'SI-13' 'SI-17']</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1190</v>
+        <v>506</v>
       </c>
       <c r="E4" t="n">
-        <v>175</v>
+        <v>79</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1470588235294118</v>
+        <v>0.1561264822134387</v>
       </c>
       <c r="G4" t="n">
-        <v>9030</v>
+        <v>6210</v>
       </c>
       <c r="H4" t="n">
-        <v>199</v>
+        <v>82</v>
       </c>
       <c r="I4" t="n">
-        <v>0.02203765227021041</v>
+        <v>0.01320450885668277</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4679144385026738</v>
+        <v>0.4906832298136646</v>
       </c>
     </row>
     <row r="5">
@@ -2357,36 +2354,35 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['CA-2' 'CA-3' 'CA-5' 'CA-6' 'CA-7' 'IR-5' 'MA-2' 'MA-3' 'PE-6' 'PE-14'
- 'PE-16' 'PL-2' 'PL-10' 'PL-11' 'PM-1' 'PM-3' 'PM-4' 'PM-6' 'PM-7' 'PM-10'
- 'PM-11' 'PM-17' 'PM-28' 'PM-31' 'PM-32' 'RA-2' 'RA-3' 'RA-6' 'RA-7'
- 'RA-9' 'RA-10' 'SA-2' 'SA-9' 'SA-23' 'SC-5' 'SC-18' 'SC-43' 'SR-2']</t>
+          <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CM-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1'
+ 'PE-1' 'PL-1' 'PM-1' 'PM-9' 'PM-18' 'PS-1' 'PS-8' 'RA-1' 'SA-1' 'SC-1'
+ 'SC-38' 'SI-1' 'SI-12' 'SR-1']</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1406</v>
+        <v>552</v>
       </c>
       <c r="E5" t="n">
-        <v>175</v>
+        <v>83</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1244665718349929</v>
+        <v>0.1503623188405797</v>
       </c>
       <c r="G5" t="n">
-        <v>9690</v>
+        <v>6456</v>
       </c>
       <c r="H5" t="n">
-        <v>251</v>
+        <v>75</v>
       </c>
       <c r="I5" t="n">
-        <v>0.02590299277605779</v>
+        <v>0.01161710037174721</v>
       </c>
       <c r="J5" t="n">
-        <v>0.4107981220657277</v>
+        <v>0.5253164556962026</v>
       </c>
     </row>
     <row r="6">
@@ -2394,39 +2390,36 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['AC-25' 'CA-8' 'CM-2' 'CM-4' 'CM-6' 'CM-7' 'CM-8' 'CM-9' 'CM-10' 'CM-12'
- 'CM-13' 'MA-6' 'PL-8' 'PL-9' 'PM-15' 'PM-16' 'PM-25' 'PM-27' 'PM-30'
- 'RA-5' 'SA-3' 'SA-4' 'SA-5' 'SA-8' 'SA-10' 'SA-11' 'SA-15' 'SA-17'
- 'SA-22' 'SC-2' 'SC-3' 'SC-4' 'SC-25' 'SC-26' 'SC-27' 'SC-29' 'SC-30'
- 'SC-32' 'SC-35' 'SC-39' 'SC-44' 'SC-49' 'SC-50' 'SI-2' 'SI-5' 'SI-6'
- 'SI-7' 'SI-16' 'SR-3' 'SR-4' 'SR-5' 'SR-6' 'SR-7' 'SR-8' 'SR-9' 'SR-10'
- 'SR-11']</t>
+          <t>['CA-5' 'CA-6' 'CA-7' 'IA-10' 'IR-5' 'MA-2' 'MA-3' 'PE-14' 'PE-16' 'PL-9'
+ 'PM-3' 'PM-4' 'PM-6' 'PM-10' 'PM-17' 'PM-28' 'PM-31' 'RA-7' 'SC-5' 'SC-7'
+ 'SC-18' 'SC-21' 'SC-22' 'SC-26' 'SC-31' 'SC-35' 'SC-40' 'SC-43' 'SC-46'
+ 'SC-48' 'SI-3' 'SI-4' 'SI-8' 'SI-11' 'SI-15' 'SR-2']</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3192</v>
+        <v>1260</v>
       </c>
       <c r="E6" t="n">
-        <v>403</v>
+        <v>139</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1262531328320802</v>
+        <v>0.1103174603174603</v>
       </c>
       <c r="G6" t="n">
-        <v>13452</v>
+        <v>9252</v>
       </c>
       <c r="H6" t="n">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0228218852215284</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="J6" t="n">
-        <v>0.5676056338028169</v>
+        <v>0.351010101010101</v>
       </c>
     </row>
     <row r="7">
@@ -2434,35 +2427,39 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['CP-2' 'CP-7' 'CP-8' 'CP-11' 'CP-12' 'CP-13' 'PE-11' 'PE-12' 'PE-13'
- 'PE-18' 'PE-19' 'PE-20' 'PE-21' 'PE-23' 'PM-8' 'SA-20' 'SC-6' 'SC-7'
- 'SC-21' 'SC-22' 'SC-24' 'SC-38' 'SC-40' 'SC-47' 'SI-8' 'SI-13' 'SI-17']</t>
+          <t>['AC-23' 'CA-2' 'CA-8' 'CM-4' 'CM-6' 'CM-7' 'CM-8' 'CM-10' 'CM-12' 'MA-6'
+ 'PL-2' 'PL-7' 'PL-8' 'PL-10' 'PL-11' 'PM-7' 'PM-11' 'PM-15' 'PM-16'
+ 'PM-25' 'PM-30' 'PM-32' 'RA-2' 'RA-3' 'RA-5' 'RA-6' 'RA-9' 'RA-10' 'SA-2'
+ 'SA-3' 'SA-4' 'SA-5' 'SA-8' 'SA-9' 'SA-10' 'SA-11' 'SA-15' 'SA-17'
+ 'SA-20' 'SA-22' 'SA-23' 'SC-2' 'SC-3' 'SC-4' 'SC-25' 'SC-27' 'SC-29'
+ 'SC-30' 'SC-32' 'SC-39' 'SC-44' 'SC-49' 'SC-50' 'SI-2' 'SI-5' 'SI-6'
+ 'SI-7' 'SR-3' 'SR-4' 'SR-5' 'SR-6' 'SR-7' 'SR-8' 'SR-9' 'SR-10' 'SR-11']</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>702</v>
+        <v>4290</v>
       </c>
       <c r="E7" t="n">
-        <v>78</v>
+        <v>485</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1111111111111111</v>
+        <v>0.1130536130536131</v>
       </c>
       <c r="G7" t="n">
-        <v>7182</v>
+        <v>14982</v>
       </c>
       <c r="H7" t="n">
-        <v>130</v>
+        <v>339</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01810080757449178</v>
+        <v>0.02262715258309972</v>
       </c>
       <c r="J7" t="n">
-        <v>0.375</v>
+        <v>0.5885922330097088</v>
       </c>
     </row>
     <row r="8">
@@ -2470,37 +2467,39 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['AC-21' 'AT-2' 'AT-3' 'AT-4' 'CP-3' 'CP-4' 'IR-2' 'IR-3' 'IR-4' 'IR-6'
- 'IR-7' 'IR-8' 'IR-9' 'MP-6' 'PE-10' 'PE-15' 'PM-5' 'PM-13' 'PM-14'
- 'PM-18' 'PM-19' 'PM-20' 'PM-21' 'PM-22' 'PM-23' 'PM-24' 'PM-26' 'PS-9'
- 'PT-2' 'PT-3' 'PT-4' 'PT-5' 'PT-6' 'PT-7' 'RA-8' 'SA-16' 'SI-18' 'SI-19'
- 'SR-12']</t>
+          <t>['AC-2' 'AC-4' 'AC-5' 'AC-6' 'AC-7' 'AC-8' 'AC-9' 'AC-11' 'AC-14' 'AC-17'
+ 'AC-18' 'AC-19' 'AC-20' 'AC-22' 'AU-2' 'AU-3' 'AU-4' 'AU-5' 'AU-6' 'AU-7'
+ 'AU-8' 'AU-11' 'AU-12' 'AU-13' 'AU-14' 'AU-16' 'CA-3' 'CA-9' 'IA-2'
+ 'IA-3' 'IA-4' 'IA-5' 'IA-6' 'IA-8' 'IA-9' 'IA-11' 'IA-12' 'MA-4' 'MA-5'
+ 'MA-7' 'MP-7' 'PE-2' 'PE-3' 'PE-5' 'PE-6' 'PE-8' 'PE-17' 'PL-4' 'PM-12'
+ 'PS-2' 'PS-3' 'PS-4' 'PS-5' 'PS-6' 'PS-7' 'SA-21' 'SC-15' 'SC-37' 'SC-41'
+ 'SC-45' 'SI-20']</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1482</v>
+        <v>3660</v>
       </c>
       <c r="E8" t="n">
-        <v>197</v>
+        <v>476</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1329284750337382</v>
+        <v>0.1300546448087432</v>
       </c>
       <c r="G8" t="n">
-        <v>9906</v>
+        <v>14152</v>
       </c>
       <c r="H8" t="n">
-        <v>164</v>
+        <v>313</v>
       </c>
       <c r="I8" t="n">
-        <v>0.01655562285483545</v>
+        <v>0.02211701526286037</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5457063711911357</v>
+        <v>0.6032953105196451</v>
       </c>
     </row>
   </sheetData>
@@ -2582,34 +2581,34 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['AC-22' 'AU-13' 'SC-2' 'SC-7' 'SC-21' 'SC-22' 'SC-25' 'SC-26' 'SC-30'
- 'SC-35' 'SC-44' 'SC-46' 'SI-14' 'SI-20' 'SI-21']</t>
+          <t>['AC-6' 'AU-13' 'CA-5' 'CA-6' 'CA-7' 'MA-3' 'PE-14' 'PM-4' 'PM-6' 'PM-10'
+ 'PM-12' 'PM-17' 'PM-28' 'PM-31' 'RA-7' 'SC-38' 'SI-20']</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>210</v>
+        <v>272</v>
       </c>
       <c r="E2" t="n">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1857142857142857</v>
+        <v>0.2242647058823529</v>
       </c>
       <c r="G2" t="n">
-        <v>4170</v>
+        <v>4692</v>
       </c>
       <c r="H2" t="n">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01726618705035971</v>
+        <v>0.03431372549019608</v>
       </c>
       <c r="J2" t="n">
-        <v>0.3513513513513514</v>
+        <v>0.2747747747747748</v>
       </c>
     </row>
     <row r="3">
@@ -2617,34 +2616,34 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['CA-5' 'CA-7' 'IR-9' 'PE-14' 'PM-3' 'PM-4' 'PM-6' 'PM-23' 'PM-27' 'PM-28'
- 'PM-31' 'PT-7' 'RA-7']</t>
+          <t>['CM-2' 'CM-3' 'CM-5' 'CM-6' 'CM-8' 'CM-9' 'CM-11' 'MA-2' 'MA-7' 'PE-16'
+ 'SC-28' 'SC-37' 'SI-10' 'SR-2']</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="E3" t="n">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="F3" t="n">
-        <v>0.25</v>
+        <v>0.3186813186813187</v>
       </c>
       <c r="G3" t="n">
-        <v>3640</v>
+        <v>3906</v>
       </c>
       <c r="H3" t="n">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03241758241758242</v>
+        <v>0.04352278545826933</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2484076433121019</v>
+        <v>0.2543859649122807</v>
       </c>
     </row>
     <row r="4">
@@ -2652,33 +2651,34 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['IR-4' 'IR-5' 'IR-6' 'IR-7' 'IR-8' 'PE-6' 'PM-16' 'PM-26' 'PT-1' 'SR-8']</t>
+          <t>['AC-5' 'AC-7' 'AC-9' 'AC-11' 'AC-14' 'AC-19' 'AU-16' 'CA-9' 'IA-2' 'IA-3'
+ 'IA-4' 'IA-5' 'IA-6' 'IA-8' 'IA-9' 'IA-10' 'IA-11' 'IA-12' 'PL-4']</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>90</v>
+        <v>342</v>
       </c>
       <c r="E4" t="n">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3444444444444444</v>
+        <v>0.2543859649122807</v>
       </c>
       <c r="G4" t="n">
-        <v>2830</v>
+        <v>5206</v>
       </c>
       <c r="H4" t="n">
-        <v>64</v>
+        <v>135</v>
       </c>
       <c r="I4" t="n">
-        <v>0.02261484098939929</v>
+        <v>0.02593161736457933</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3263157894736842</v>
+        <v>0.3918918918918919</v>
       </c>
     </row>
     <row r="5">
@@ -2686,34 +2686,33 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>['PE-8' 'PL-2' 'PL-10' 'PL-11' 'PM-1' 'PM-7' 'PM-11' 'PM-32' 'RA-2' 'RA-3'
- 'RA-9' 'SA-8' 'SA-20' 'SA-23' 'SC-38' 'SR-2' 'SR-7']</t>
+          <t>['AC-18' 'AC-21' 'PE-17' 'PE-19' 'PE-21' 'SC-15' 'SC-18' 'SC-43']</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>272</v>
+        <v>56</v>
       </c>
       <c r="E5" t="n">
-        <v>76</v>
+        <v>10</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2794117647058824</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="G5" t="n">
-        <v>4692</v>
+        <v>2280</v>
       </c>
       <c r="H5" t="n">
-        <v>147</v>
+        <v>38</v>
       </c>
       <c r="I5" t="n">
-        <v>0.03132992327365729</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="J5" t="n">
-        <v>0.3408071748878924</v>
+        <v>0.2083333333333333</v>
       </c>
     </row>
     <row r="6">
@@ -2721,35 +2720,34 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['AC-3' 'AC-23' 'CM-12' 'CM-13' 'PM-2' 'PM-5' 'PM-20' 'PM-21' 'PM-22'
- 'PM-24' 'PT-2' 'PT-3' 'PT-4' 'PT-5' 'PT-6' 'PT-8' 'RA-8' 'SC-4' 'SC-42'
- 'SI-18' 'SI-19']</t>
+          <t>['CA-2' 'CA-8' 'CM-4' 'PM-15' 'RA-5' 'RA-6' 'RA-10' 'SA-11' 'SI-2' 'SI-5'
+ 'SI-6']</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>420</v>
+        <v>110</v>
       </c>
       <c r="E6" t="n">
-        <v>95</v>
+        <v>40</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2261904761904762</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="G6" t="n">
-        <v>5712</v>
+        <v>3102</v>
       </c>
       <c r="H6" t="n">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="I6" t="n">
-        <v>0.02293417366946779</v>
+        <v>0.02578981302385558</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4203539823008849</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="7">
@@ -2757,34 +2755,34 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['PE-5' 'PE-18' 'PE-19' 'PE-20' 'PE-21' 'PE-23' 'PM-8' 'SC-5' 'SC-6'
- 'SC-40' 'SI-8']</t>
+          <t>['PM-1' 'PM-18' 'PM-19' 'PM-29' 'PM-30' 'SA-23' 'SR-4' 'SR-7' 'SR-8'
+ 'SR-9' 'SR-10' 'SR-11']</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="E7" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1727272727272727</v>
+        <v>0.1742424242424243</v>
       </c>
       <c r="G7" t="n">
-        <v>3102</v>
+        <v>3372</v>
       </c>
       <c r="H7" t="n">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="I7" t="n">
-        <v>0.01063829787234043</v>
+        <v>0.01749703440094899</v>
       </c>
       <c r="J7" t="n">
-        <v>0.3653846153846154</v>
+        <v>0.2804878048780488</v>
       </c>
     </row>
     <row r="8">
@@ -2792,34 +2790,35 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['CM-2' 'CM-4' 'CM-7' 'CM-8' 'CM-9' 'CM-10' 'CM-11' 'PM-15' 'RA-5' 'SA-10'
- 'SC-3' 'SI-2' 'SI-5']</t>
+          <t>['AC-23' 'CM-12' 'IR-7' 'IR-8' 'PM-5' 'PM-20' 'PM-21' 'PM-22' 'PM-23'
+ 'PM-24' 'PM-26' 'PT-1' 'PT-2' 'PT-3' 'PT-4' 'PT-5' 'PT-6' 'PT-7' 'SC-42'
+ 'SI-18' 'SI-19']</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>156</v>
+        <v>420</v>
       </c>
       <c r="E8" t="n">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3717948717948718</v>
+        <v>0.1952380952380952</v>
       </c>
       <c r="G8" t="n">
-        <v>3640</v>
+        <v>5712</v>
       </c>
       <c r="H8" t="n">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="I8" t="n">
-        <v>0.04010989010989011</v>
+        <v>0.01680672268907563</v>
       </c>
       <c r="J8" t="n">
-        <v>0.2843137254901961</v>
+        <v>0.4606741573033708</v>
       </c>
     </row>
     <row r="9">
@@ -2827,35 +2826,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['AC-8' 'AU-2' 'AU-3' 'AU-6' 'AU-7' 'AU-12' 'CM-3' 'CM-5' 'CM-6' 'PL-9'
- 'SC-18' 'SC-28' 'SC-31' 'SC-34' 'SC-37' 'SC-48' 'SI-3' 'SI-4' 'SI-7'
- 'SI-10' 'SI-11' 'SI-15']</t>
+          <t>['CP-12' 'IR-4' 'IR-5' 'IR-6' 'PM-16' 'SC-5' 'SC-6' 'SC-7' 'SC-24' 'SC-25'
+ 'SC-26' 'SC-30' 'SC-35' 'SC-44' 'SI-17']</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>462</v>
+        <v>210</v>
       </c>
       <c r="E9" t="n">
-        <v>141</v>
+        <v>46</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3051948051948052</v>
+        <v>0.219047619047619</v>
       </c>
       <c r="G9" t="n">
-        <v>5962</v>
+        <v>4170</v>
       </c>
       <c r="H9" t="n">
-        <v>241</v>
+        <v>110</v>
       </c>
       <c r="I9" t="n">
-        <v>0.04042267695404227</v>
+        <v>0.026378896882494</v>
       </c>
       <c r="J9" t="n">
-        <v>0.369109947643979</v>
+        <v>0.2948717948717949</v>
       </c>
     </row>
     <row r="10">
@@ -2863,33 +2861,34 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['CP-4' 'CP-7' 'CP-9' 'PE-11' 'PE-12' 'PE-17' 'SC-32' 'SC-36']</t>
+          <t>['AC-2' 'MA-5' 'MP-2' 'PE-2' 'PE-3' 'PE-4' 'PE-5' 'PE-9' 'PS-2' 'PS-3'
+ 'PS-4' 'PS-5' 'PS-6' 'PS-7' 'SA-21']</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>56</v>
+        <v>210</v>
       </c>
       <c r="E10" t="n">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3035714285714285</v>
+        <v>0.3904761904761905</v>
       </c>
       <c r="G10" t="n">
-        <v>2280</v>
+        <v>4170</v>
       </c>
       <c r="H10" t="n">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="I10" t="n">
-        <v>0.02412280701754386</v>
+        <v>0.02613908872901679</v>
       </c>
       <c r="J10" t="n">
-        <v>0.2361111111111111</v>
+        <v>0.4293193717277487</v>
       </c>
     </row>
     <row r="11">
@@ -2897,34 +2896,34 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['AC-14' 'AC-21' 'AU-16' 'IA-2' 'IA-4' 'IA-5' 'IA-6' 'IA-8' 'IA-9' 'IA-10'
- 'IA-11' 'IA-12' 'SC-15' 'SC-45']</t>
+          <t>['CM-13' 'PE-18' 'PE-20' 'PE-23' 'PL-2' 'PL-10' 'PL-11' 'PM-8' 'PM-11'
+ 'PM-27' 'PM-32' 'RA-2' 'RA-3' 'RA-8' 'RA-9']</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="E11" t="n">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2527472527472527</v>
+        <v>0.2714285714285714</v>
       </c>
       <c r="G11" t="n">
-        <v>3906</v>
+        <v>4170</v>
       </c>
       <c r="H11" t="n">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="I11" t="n">
-        <v>0.02124935995903738</v>
+        <v>0.02446043165467626</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3565891472868217</v>
+        <v>0.3584905660377358</v>
       </c>
     </row>
     <row r="12">
@@ -2932,34 +2931,34 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['AT-2' 'AT-3' 'AT-4' 'CP-3' 'IR-2' 'IR-3' 'PE-2' 'PE-10' 'PE-15' 'PM-12'
- 'PM-13' 'PM-14' 'PS-4' 'PS-5' 'PS-9']</t>
+          <t>['AC-10' 'AC-12' 'PL-9' 'SC-10' 'SC-11' 'SC-23' 'SI-3' 'SI-8' 'SI-11'
+ 'SI-15']</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>210</v>
+        <v>90</v>
       </c>
       <c r="E12" t="n">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="F12" t="n">
-        <v>0.2619047619047619</v>
+        <v>0.1888888888888889</v>
       </c>
       <c r="G12" t="n">
-        <v>4170</v>
+        <v>2830</v>
       </c>
       <c r="H12" t="n">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="I12" t="n">
-        <v>0.02326139088729017</v>
+        <v>0.01448763250883392</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3618421052631579</v>
+        <v>0.293103448275862</v>
       </c>
     </row>
     <row r="13">
@@ -2967,34 +2966,34 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['AC-2' 'AC-9' 'AC-11' 'AC-17' 'AC-20' 'CA-3' 'MP-7' 'PL-4' 'PS-2' 'PS-3'
- 'PS-6' 'PS-7' 'SA-21' 'SC-41']</t>
+          <t>['AC-3' 'AC-4' 'AC-16' 'AC-25' 'MP-3' 'PE-22' 'PM-2' 'PT-8' 'SC-2' 'SC-3'
+ 'SC-4' 'SC-31' 'SC-32' 'SC-39' 'SC-46' 'SC-49' 'SC-50' 'SI-16']</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>182</v>
+        <v>306</v>
       </c>
       <c r="E13" t="n">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="F13" t="n">
-        <v>0.3076923076923077</v>
+        <v>0.2091503267973856</v>
       </c>
       <c r="G13" t="n">
-        <v>3906</v>
+        <v>4950</v>
       </c>
       <c r="H13" t="n">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="I13" t="n">
-        <v>0.03097798259088582</v>
+        <v>0.02606060606060606</v>
       </c>
       <c r="J13" t="n">
-        <v>0.3163841807909605</v>
+        <v>0.3316062176165803</v>
       </c>
     </row>
     <row r="14">
@@ -3002,34 +3001,34 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['AC-24' 'AU-4' 'AU-5' 'AU-8' 'AU-9' 'AU-10' 'AU-11' 'AU-14' 'SC-8'
- 'SC-13' 'SC-16' 'SC-20']</t>
+          <t>['PL-7' 'PL-8' 'PM-3' 'PM-7' 'SA-2' 'SA-3' 'SA-4' 'SA-5' 'SA-9' 'SA-17'
+ 'SA-22' 'SC-27' 'SC-29' 'SR-3' 'SR-5']</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>132</v>
+        <v>210</v>
       </c>
       <c r="E14" t="n">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3095238095238095</v>
       </c>
       <c r="G14" t="n">
-        <v>3372</v>
+        <v>4170</v>
       </c>
       <c r="H14" t="n">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="I14" t="n">
-        <v>0.02787663107947806</v>
+        <v>0.02997601918465228</v>
       </c>
       <c r="J14" t="n">
-        <v>0.3188405797101449</v>
+        <v>0.3421052631578947</v>
       </c>
     </row>
     <row r="15">
@@ -3037,34 +3036,34 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['CP-2' 'CP-6' 'CP-8' 'CP-10' 'CP-11' 'CP-12' 'CP-13' 'MP-2' 'MP-4' 'PE-3'
- 'PE-4' 'PE-9' 'PE-13' 'SC-24' 'SC-47' 'SI-13' 'SI-17']</t>
+          <t>['AC-8' 'AC-17' 'AU-2' 'AU-3' 'AU-4' 'AU-5' 'AU-6' 'AU-7' 'AU-8' 'AU-9'
+ 'AU-11' 'AU-12' 'AU-14' 'MA-4' 'PE-6' 'SC-45' 'SC-48' 'SI-4']</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>272</v>
+        <v>306</v>
       </c>
       <c r="E15" t="n">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="F15" t="n">
-        <v>0.2426470588235294</v>
+        <v>0.3954248366013072</v>
       </c>
       <c r="G15" t="n">
-        <v>4692</v>
+        <v>4950</v>
       </c>
       <c r="H15" t="n">
-        <v>114</v>
+        <v>183</v>
       </c>
       <c r="I15" t="n">
-        <v>0.02429667519181586</v>
+        <v>0.03696969696969697</v>
       </c>
       <c r="J15" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.3980263157894737</v>
       </c>
     </row>
     <row r="16">
@@ -3072,33 +3071,34 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['AC-5' 'AC-6' 'MA-2' 'MA-3' 'MA-4' 'MA-5' 'MA-7' 'MP-6' 'PE-16' 'SR-12']</t>
+          <t>['AC-24' 'AU-10' 'IA-7' 'SC-8' 'SC-12' 'SC-13' 'SC-16' 'SC-17' 'SC-20'
+ 'SC-21' 'SC-22' 'SC-40']</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="E16" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G16" t="n">
-        <v>2830</v>
+        <v>3372</v>
       </c>
       <c r="H16" t="n">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="I16" t="n">
-        <v>0.03604240282685512</v>
+        <v>0.02075919335705812</v>
       </c>
       <c r="J16" t="n">
-        <v>0.2444444444444444</v>
+        <v>0.3859649122807017</v>
       </c>
     </row>
     <row r="17">
@@ -3106,34 +3106,34 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['MA-6' 'PL-7' 'PL-8' 'PM-30' 'SA-2' 'SA-3' 'SA-4' 'SA-5' 'SA-9' 'SA-15'
- 'SA-16' 'SA-17' 'SA-22' 'SR-3' 'SR-4' 'SR-5' 'SR-9' 'SR-10' 'SR-11']</t>
+          <t>['CM-7' 'CM-10' 'CM-14' 'PE-8' 'PM-25' 'SA-8' 'SA-10' 'SA-15' 'SA-20'
+ 'SI-1' 'SI-7' 'SR-6']</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>342</v>
+        <v>132</v>
       </c>
       <c r="E17" t="n">
-        <v>108</v>
+        <v>35</v>
       </c>
       <c r="F17" t="n">
-        <v>0.3157894736842105</v>
+        <v>0.2651515151515151</v>
       </c>
       <c r="G17" t="n">
-        <v>5206</v>
+        <v>3372</v>
       </c>
       <c r="H17" t="n">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="I17" t="n">
-        <v>0.03054168267383788</v>
+        <v>0.04626334519572953</v>
       </c>
       <c r="J17" t="n">
-        <v>0.4044943820224719</v>
+        <v>0.1832460732984293</v>
       </c>
     </row>
     <row r="18">
@@ -3141,34 +3141,33 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>['AC-10' 'AC-12' 'AC-16' 'AC-25' 'CM-14' 'IA-7' 'SC-10' 'SC-11' 'SC-12'
- 'SC-17' 'SC-23' 'SC-39' 'SI-16']</t>
+          <t>['AC-20' 'CA-3' 'MP-6' 'MP-7' 'SC-34' 'SC-41' 'SI-14' 'SI-21' 'SR-12']</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>156</v>
+        <v>72</v>
       </c>
       <c r="E18" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1730769230769231</v>
+        <v>0.2222222222222222</v>
       </c>
       <c r="G18" t="n">
-        <v>3640</v>
+        <v>2556</v>
       </c>
       <c r="H18" t="n">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I18" t="n">
-        <v>0.01565934065934066</v>
+        <v>0.02034428794992175</v>
       </c>
       <c r="J18" t="n">
-        <v>0.3214285714285715</v>
+        <v>0.2352941176470588</v>
       </c>
     </row>
     <row r="19">
@@ -3176,34 +3175,34 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['AC-4' 'AC-7' 'AC-18' 'AC-19' 'CA-9' 'IA-3' 'MP-3' 'MP-5' 'PE-22' 'SC-27'
- 'SC-29' 'SC-43' 'SC-49' 'SC-50']</t>
+          <t>['AC-22' 'AT-2' 'AT-3' 'AT-4' 'CP-3' 'CP-4' 'IR-2' 'IR-3' 'IR-9' 'PE-10'
+ 'PE-15' 'PM-13' 'PM-14' 'PS-9' 'SA-16']</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="E19" t="n">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2142857142857143</v>
+        <v>0.2952380952380952</v>
       </c>
       <c r="G19" t="n">
-        <v>3906</v>
+        <v>4170</v>
       </c>
       <c r="H19" t="n">
-        <v>113</v>
+        <v>72</v>
       </c>
       <c r="I19" t="n">
-        <v>0.02892985151049667</v>
+        <v>0.01726618705035971</v>
       </c>
       <c r="J19" t="n">
-        <v>0.2565789473684211</v>
+        <v>0.4626865671641791</v>
       </c>
     </row>
     <row r="20">
@@ -3211,34 +3210,34 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['CA-2' 'CA-6' 'CA-8' 'PM-10' 'PM-17' 'PM-19' 'PM-25' 'PM-29' 'RA-6'
- 'RA-10' 'SA-11' 'SI-6' 'SR-6']</t>
+          <t>['CP-2' 'CP-6' 'CP-7' 'CP-8' 'CP-9' 'CP-10' 'CP-11' 'CP-13' 'MA-6' 'MP-4'
+ 'MP-5' 'PE-11' 'PE-12' 'PE-13' 'SC-36' 'SC-47' 'SI-13']</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>156</v>
+        <v>272</v>
       </c>
       <c r="E20" t="n">
-        <v>22</v>
+        <v>81</v>
       </c>
       <c r="F20" t="n">
-        <v>0.141025641025641</v>
+        <v>0.2977941176470588</v>
       </c>
       <c r="G20" t="n">
-        <v>3640</v>
+        <v>4692</v>
       </c>
       <c r="H20" t="n">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="I20" t="n">
-        <v>0.01868131868131868</v>
+        <v>0.02003410059676044</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2444444444444444</v>
+        <v>0.4628571428571429</v>
       </c>
     </row>
     <row r="21">
@@ -3246,35 +3245,34 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
           <t>['AC-1' 'AT-1' 'AU-1' 'CA-1' 'CM-1' 'CP-1' 'IA-1' 'IR-1' 'MA-1' 'MP-1'
- 'PE-1' 'PL-1' 'PM-9' 'PM-18' 'PS-1' 'PS-8' 'RA-1' 'SA-1' 'SC-1' 'SI-1'
- 'SI-12' 'SR-1']</t>
+ 'PE-1' 'PL-1' 'PM-9' 'PS-1' 'PS-8' 'RA-1' 'SA-1' 'SC-1' 'SI-12' 'SR-1']</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>462</v>
+        <v>380</v>
       </c>
       <c r="E21" t="n">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1688311688311688</v>
+        <v>0.1894736842105263</v>
       </c>
       <c r="G21" t="n">
-        <v>5962</v>
+        <v>5460</v>
       </c>
       <c r="H21" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I21" t="n">
-        <v>0.01056692385105669</v>
+        <v>0.01135531135531135</v>
       </c>
       <c r="J21" t="n">
-        <v>0.5531914893617021</v>
+        <v>0.5373134328358209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>